<commit_message>
Updated Export Formatting and Added Hold - Stray Data
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Outcomes</t>
   </si>
@@ -92,6 +92,54 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Animal ID</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Review Date</t>
+  </si>
+  <si>
+    <t>A0058484847</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 234, Cage 3</t>
+  </si>
+  <si>
+    <t>2025-05-16</t>
+  </si>
+  <si>
+    <t>A0058484864</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 234, Cage 4</t>
+  </si>
+  <si>
+    <t>A0058457661</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Treatment, 02</t>
+  </si>
+  <si>
+    <t>A0058467665</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Small Animals &amp; Exotics, Bird Cage 2</t>
+  </si>
+  <si>
+    <t>2025-05-15</t>
+  </si>
+  <si>
+    <t>A0058480470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Small Animals &amp; Exotics, Bird Cage 4</t>
+  </si>
+  <si>
+    <t>2025-05-19</t>
   </si>
 </sst>
 </file>
@@ -438,7 +486,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -472,107 +520,107 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>6</v>
       </c>
     </row>
@@ -603,7 +651,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>16</v>
@@ -636,7 +684,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24">
         <v>15</v>
@@ -651,6 +699,72 @@
       </c>
       <c r="C25">
         <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated morning_report.py to prompt for dates wanted, added readme.txt, and improved functionality
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Morning Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Intake Count Detail" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="128">
   <si>
     <t>Outcomes</t>
   </si>
@@ -22,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (previous business day)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (previous business day)</t>
+    <t>Adoptions (05/23/2025, 05/24/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (05/23/2025, 05/24/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -103,50 +104,311 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>A0058484847</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 234, Cage 3</t>
-  </si>
-  <si>
-    <t>2025-05-16</t>
-  </si>
-  <si>
-    <t>A0058484864</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 234, Cage 4</t>
-  </si>
-  <si>
-    <t>A0058457661</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Treatment, 02</t>
-  </si>
-  <si>
-    <t>A0058467665</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Small Animals &amp; Exotics, Bird Cage 2</t>
-  </si>
-  <si>
-    <t>2025-05-15</t>
-  </si>
-  <si>
-    <t>A0058480470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Small Animals &amp; Exotics, Bird Cage 4</t>
-  </si>
-  <si>
-    <t>2025-05-19</t>
+    <t>A0058531162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 234, Cage 1</t>
+  </si>
+  <si>
+    <t>2025-05-23</t>
+  </si>
+  <si>
+    <t>A0058549222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Farm, Stall #3</t>
+  </si>
+  <si>
+    <t>2025-05-28</t>
+  </si>
+  <si>
+    <t>A0058553591</t>
+  </si>
+  <si>
+    <t>2025-05-29</t>
+  </si>
+  <si>
+    <t>A0058561257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 08</t>
+  </si>
+  <si>
+    <t>2025-05-27</t>
+  </si>
+  <si>
+    <t>A0058571055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 227, Mammal 1</t>
+  </si>
+  <si>
+    <t>2025-05-30</t>
+  </si>
+  <si>
+    <t>A0058573503</t>
+  </si>
+  <si>
+    <t>No Review Date</t>
+  </si>
+  <si>
+    <t>A0058521446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Multi Animal Holding</t>
+  </si>
+  <si>
+    <t>A0058564519</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Receiving, Receiving</t>
+  </si>
+  <si>
+    <t>A0058571051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Small Animals &amp; Exotics, Mammal 1</t>
+  </si>
+  <si>
+    <t>A0058571053</t>
+  </si>
+  <si>
+    <t>A0058571057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Small Animals &amp; Exotics, Mammal 2</t>
+  </si>
+  <si>
+    <t>AnimalNumber</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>textbox44</t>
+  </si>
+  <si>
+    <t>OperationType</t>
+  </si>
+  <si>
+    <t>OperationSubType</t>
+  </si>
+  <si>
+    <t>IntakeGroup</t>
+  </si>
+  <si>
+    <t>A0050101337</t>
+  </si>
+  <si>
+    <t>A0058549497</t>
+  </si>
+  <si>
+    <t>A0058561749</t>
+  </si>
+  <si>
+    <t>A0058563982</t>
+  </si>
+  <si>
+    <t>A0023291294</t>
+  </si>
+  <si>
+    <t>A0052971516</t>
+  </si>
+  <si>
+    <t>A0058489875</t>
+  </si>
+  <si>
+    <t>A0058564798</t>
+  </si>
+  <si>
+    <t>A0058553595</t>
+  </si>
+  <si>
+    <t>A0058561734</t>
+  </si>
+  <si>
+    <t>A0058561745</t>
+  </si>
+  <si>
+    <t>A0058561748</t>
+  </si>
+  <si>
+    <t>A0058561752</t>
+  </si>
+  <si>
+    <t>A0058562068</t>
+  </si>
+  <si>
+    <t>A0058563025</t>
+  </si>
+  <si>
+    <t>A0058568632</t>
+  </si>
+  <si>
+    <t>A0058569854</t>
+  </si>
+  <si>
+    <t>A0058569856</t>
+  </si>
+  <si>
+    <t>A0058569859</t>
+  </si>
+  <si>
+    <t>A0058569861</t>
+  </si>
+  <si>
+    <t>A0058571047</t>
+  </si>
+  <si>
+    <t>A0058553982</t>
+  </si>
+  <si>
+    <t>A0058553986</t>
+  </si>
+  <si>
+    <t>A0058561031</t>
+  </si>
+  <si>
+    <t>A0058561034</t>
+  </si>
+  <si>
+    <t>Mammal</t>
+  </si>
+  <si>
+    <t>Farm Type Fowl</t>
+  </si>
+  <si>
+    <t>Rodent</t>
+  </si>
+  <si>
+    <t>Clinic</t>
+  </si>
+  <si>
+    <t>Owner/Guardian Surrender</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Seized / Custody</t>
+  </si>
+  <si>
+    <t>Stray</t>
+  </si>
+  <si>
+    <t>Transfer In</t>
+  </si>
+  <si>
+    <t>Case Assistance</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - FIELD!</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>ACO or DCO in County</t>
+  </si>
+  <si>
+    <t>Feral Cat Focus</t>
+  </si>
+  <si>
+    <t>Clinic - Case Assistance</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
+  </si>
+  <si>
+    <t>Clinic - Retention</t>
+  </si>
+  <si>
+    <t>Clinic - Case Assistance - Outreach</t>
+  </si>
+  <si>
+    <t>Clinic - Outreach</t>
+  </si>
+  <si>
+    <t>Boarder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +419,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -177,7 +447,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -185,13 +455,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +775,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -509,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -517,7 +806,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -533,7 +822,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -549,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -557,7 +846,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -573,7 +862,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -589,7 +878,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -597,7 +886,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -605,7 +894,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -613,7 +902,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -621,7 +910,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -640,7 +929,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C20">
         <v>29</v>
@@ -651,10 +940,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -662,10 +951,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>76</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -673,10 +962,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C23">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -684,10 +973,10 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -695,10 +984,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="C25">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -731,40 +1020,970 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59">
+        <v>8</v>
+      </c>
+      <c r="D59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="C32" t="s">
-        <v>41</v>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="3">
+        <v>45801</v>
+      </c>
+      <c r="D29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D30" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45800</v>
+      </c>
+      <c r="D33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed logic for how Field Euths are categorized in intake sheet
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="108">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (05/23/2025, 05/24/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (05/23/2025, 05/24/2025)</t>
+    <t>Adoptions (06/06/2025, 06/07/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/06/2025, 06/07/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,79 +104,61 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>A0058531162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 234, Cage 1</t>
-  </si>
-  <si>
-    <t>2025-05-23</t>
-  </si>
-  <si>
-    <t>A0058549222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Farm, Stall #3</t>
-  </si>
-  <si>
-    <t>2025-05-28</t>
-  </si>
-  <si>
-    <t>A0058553591</t>
-  </si>
-  <si>
-    <t>2025-05-29</t>
-  </si>
-  <si>
-    <t>A0058561257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 08</t>
-  </si>
-  <si>
-    <t>2025-05-27</t>
-  </si>
-  <si>
-    <t>A0058571055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Multi-Animal Holding, Room 227, Mammal 1</t>
-  </si>
-  <si>
-    <t>2025-05-30</t>
-  </si>
-  <si>
-    <t>A0058573503</t>
-  </si>
-  <si>
-    <t>No Review Date</t>
-  </si>
-  <si>
-    <t>A0058521446</t>
+    <t>A0058650379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Treatment, 02</t>
+  </si>
+  <si>
+    <t>2025-06-10</t>
+  </si>
+  <si>
+    <t>A0058662816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Treatment, 04</t>
+  </si>
+  <si>
+    <t>2025-06-12</t>
+  </si>
+  <si>
+    <t>A0058648104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Farm, Farm</t>
+  </si>
+  <si>
+    <t>2025-06-11</t>
+  </si>
+  <si>
+    <t>A0058636089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 04 - A</t>
+  </si>
+  <si>
+    <t>2025-06-09</t>
+  </si>
+  <si>
+    <t>A0058639310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 01 - B</t>
+  </si>
+  <si>
+    <t>A0058627436</t>
   </si>
   <si>
     <t xml:space="preserve">  Multi-Animal Holding, Room 229, Multi Animal Holding</t>
   </si>
   <si>
-    <t>A0058564519</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Receiving, Receiving</t>
-  </si>
-  <si>
-    <t>A0058571051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Small Animals &amp; Exotics, Mammal 1</t>
-  </si>
-  <si>
-    <t>A0058571053</t>
-  </si>
-  <si>
-    <t>A0058571057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Small Animals &amp; Exotics, Mammal 2</t>
+    <t>A0058662527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 1</t>
+  </si>
+  <si>
+    <t>2025-06-13</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -197,88 +179,46 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0050101337</t>
-  </si>
-  <si>
-    <t>A0058549497</t>
-  </si>
-  <si>
-    <t>A0058561749</t>
-  </si>
-  <si>
-    <t>A0058563982</t>
-  </si>
-  <si>
-    <t>A0023291294</t>
-  </si>
-  <si>
-    <t>A0052971516</t>
-  </si>
-  <si>
-    <t>A0058489875</t>
-  </si>
-  <si>
-    <t>A0058564798</t>
-  </si>
-  <si>
-    <t>A0058553595</t>
-  </si>
-  <si>
-    <t>A0058561734</t>
-  </si>
-  <si>
-    <t>A0058561745</t>
-  </si>
-  <si>
-    <t>A0058561748</t>
-  </si>
-  <si>
-    <t>A0058561752</t>
-  </si>
-  <si>
-    <t>A0058562068</t>
-  </si>
-  <si>
-    <t>A0058563025</t>
-  </si>
-  <si>
-    <t>A0058568632</t>
-  </si>
-  <si>
-    <t>A0058569854</t>
-  </si>
-  <si>
-    <t>A0058569856</t>
-  </si>
-  <si>
-    <t>A0058569859</t>
-  </si>
-  <si>
-    <t>A0058569861</t>
-  </si>
-  <si>
-    <t>A0058571047</t>
-  </si>
-  <si>
-    <t>A0058553982</t>
-  </si>
-  <si>
-    <t>A0058553986</t>
-  </si>
-  <si>
-    <t>A0058561031</t>
-  </si>
-  <si>
-    <t>A0058561034</t>
-  </si>
-  <si>
-    <t>Mammal</t>
-  </si>
-  <si>
-    <t>Farm Type Fowl</t>
-  </si>
-  <si>
-    <t>Rodent</t>
+    <t>A0058467398</t>
+  </si>
+  <si>
+    <t>A0058467403</t>
+  </si>
+  <si>
+    <t>A0058553460</t>
+  </si>
+  <si>
+    <t>A0058620400</t>
+  </si>
+  <si>
+    <t>A0058654136</t>
+  </si>
+  <si>
+    <t>A0057976477</t>
+  </si>
+  <si>
+    <t>A0058656259</t>
+  </si>
+  <si>
+    <t>A0058656084</t>
+  </si>
+  <si>
+    <t>A0058656088</t>
+  </si>
+  <si>
+    <t>A0058657306</t>
+  </si>
+  <si>
+    <t>A0058654163</t>
+  </si>
+  <si>
+    <t>A0058654173</t>
+  </si>
+  <si>
+    <t>Domestic (Cage) Bird</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
   </si>
   <si>
     <t>Clinic</t>
@@ -299,97 +239,97 @@
     <t>Transfer In</t>
   </si>
   <si>
-    <t>Case Assistance</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - FIELD!</t>
+    <t>Medical Treatment</t>
   </si>
   <si>
     <t>Euthanasia Request - OTC!</t>
   </si>
   <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>Medical Treatment - OTC!</t>
+  </si>
+  <si>
     <t>Signed Over</t>
   </si>
   <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
     <t>Field</t>
   </si>
   <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>ACO or DCO in County</t>
-  </si>
-  <si>
-    <t>Feral Cat Focus</t>
+    <t>Shelter out Coalit. (Not SPCA)</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Retention</t>
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
-  </si>
-  <si>
-    <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
-  </si>
-  <si>
-    <t>Clinic - Retention</t>
   </si>
   <si>
     <t>Clinic - Case Assistance - Outreach</t>
@@ -775,7 +715,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -798,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -822,7 +762,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -830,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -838,7 +778,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -846,7 +786,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -862,7 +802,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -870,7 +810,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -878,7 +818,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -886,7 +826,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -894,7 +834,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -910,7 +850,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -929,10 +869,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C20">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -940,10 +880,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C21">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -951,10 +891,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C22">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -962,10 +902,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C23">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -973,10 +913,10 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -984,10 +924,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C25">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1028,32 +968,32 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
         <v>40</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1061,10 +1001,10 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1075,242 +1015,186 @@
         <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
         <v>47</v>
       </c>
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" t="s">
-        <v>42</v>
+      <c r="A37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" t="s">
-        <v>42</v>
+        <v>73</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>23</v>
+      <c r="A41" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>105</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>107</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>87</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>70</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>72</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>86</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B59">
-        <v>8</v>
-      </c>
-      <c r="D59">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>103</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1320,7 +1204,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1328,662 +1212,302 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3">
-        <v>45801</v>
+        <v>45814</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
-        <v>45801</v>
+        <v>45814</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C12" s="3">
-        <v>45800</v>
+        <v>45815</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45800</v>
+        <v>45815</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="3">
-        <v>45800</v>
-      </c>
-      <c r="D16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
         <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="3">
-        <v>45800</v>
-      </c>
-      <c r="D17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" t="s">
-        <v>99</v>
-      </c>
-      <c r="F17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="3">
-        <v>45800</v>
-      </c>
-      <c r="D18" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="3">
-        <v>45800</v>
-      </c>
-      <c r="D19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D22" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D25" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D28" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="3">
-        <v>45801</v>
-      </c>
-      <c r="D29" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="3">
-        <v>45800</v>
-      </c>
-      <c r="D30" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="3">
-        <v>45800</v>
-      </c>
-      <c r="D31" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="3">
-        <v>45800</v>
-      </c>
-      <c r="D32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" t="s">
-        <v>102</v>
-      </c>
-      <c r="F32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="3">
-        <v>45800</v>
-      </c>
-      <c r="D33" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F33" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated load files for the day
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="114">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/06/2025, 06/07/2025, 06/08/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/06/2025, 06/07/2025, 06/08/2025)</t>
+    <t>Adoptions (06/09/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/09/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,6 +104,15 @@
     <t>Review Date</t>
   </si>
   <si>
+    <t>A0058670106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 231, Cage 5</t>
+  </si>
+  <si>
+    <t>2025-06-13</t>
+  </si>
+  <si>
     <t>A0058650379</t>
   </si>
   <si>
@@ -122,6 +131,12 @@
     <t>2025-06-12</t>
   </si>
   <si>
+    <t>A0058673429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Treatment, 05 - B</t>
+  </si>
+  <si>
     <t>A0058648104</t>
   </si>
   <si>
@@ -131,19 +146,13 @@
     <t>2025-06-11</t>
   </si>
   <si>
-    <t>A0058636089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 04 - A</t>
-  </si>
-  <si>
-    <t>2025-06-09</t>
-  </si>
-  <si>
-    <t>A0058639310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 01 - B</t>
+    <t>A0058672310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Farm, Stall #3</t>
+  </si>
+  <si>
+    <t>2025-06-16</t>
   </si>
   <si>
     <t>A0058627436</t>
@@ -158,7 +167,10 @@
     <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 1</t>
   </si>
   <si>
-    <t>2025-06-13</t>
+    <t>A0058676024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Receiving, Receiving</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -179,154 +191,160 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058467398</t>
-  </si>
-  <si>
-    <t>A0058467403</t>
-  </si>
-  <si>
-    <t>A0058553460</t>
-  </si>
-  <si>
-    <t>A0058620400</t>
-  </si>
-  <si>
-    <t>A0058654136</t>
-  </si>
-  <si>
-    <t>A0057976477</t>
-  </si>
-  <si>
-    <t>A0058656259</t>
-  </si>
-  <si>
-    <t>A0058656084</t>
-  </si>
-  <si>
-    <t>A0058656088</t>
-  </si>
-  <si>
-    <t>A0058657306</t>
-  </si>
-  <si>
-    <t>A0058654163</t>
-  </si>
-  <si>
-    <t>A0058654173</t>
-  </si>
-  <si>
-    <t>Domestic (Cage) Bird</t>
+    <t>A0058360707</t>
+  </si>
+  <si>
+    <t>A0058360718</t>
+  </si>
+  <si>
+    <t>A0058360725</t>
+  </si>
+  <si>
+    <t>A0058668717</t>
+  </si>
+  <si>
+    <t>A0058669677</t>
+  </si>
+  <si>
+    <t>A0058670777</t>
+  </si>
+  <si>
+    <t>A0058670802</t>
+  </si>
+  <si>
+    <t>A0058670807</t>
+  </si>
+  <si>
+    <t>A0058671983</t>
+  </si>
+  <si>
+    <t>A0058672839</t>
+  </si>
+  <si>
+    <t>A0032144299</t>
+  </si>
+  <si>
+    <t>A0058669457</t>
+  </si>
+  <si>
+    <t>A0058669458</t>
   </si>
   <si>
     <t>Rabbit</t>
   </si>
   <si>
+    <t>Farm Type Fowl</t>
+  </si>
+  <si>
+    <t>Reptile/Amphibian</t>
+  </si>
+  <si>
     <t>Clinic</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Seized / Custody</t>
+  </si>
+  <si>
+    <t>Stray</t>
+  </si>
+  <si>
+    <t>Retention</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - FIELD!</t>
+  </si>
+  <si>
+    <t>Protective Custody</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>Abandoned/Dumped Off at SPCA</t>
+  </si>
+  <si>
+    <t>Clinic - Retention</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>not counted</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Transfer In</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
     <t>Return</t>
   </si>
   <si>
-    <t>Seized / Custody</t>
-  </si>
-  <si>
-    <t>Stray</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>Medical Treatment</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>Medical Treatment - OTC!</t>
-  </si>
-  <si>
-    <t>Signed Over</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Shelter out Coalit. (Not SPCA)</t>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
   </si>
   <si>
     <t>Clinic - Stray</t>
-  </si>
-  <si>
-    <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
-  </si>
-  <si>
-    <t>Clinic - Retention</t>
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
@@ -715,7 +733,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -738,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -746,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -762,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -778,7 +796,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -802,7 +820,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -810,7 +828,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -818,7 +836,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -826,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -850,7 +868,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -880,7 +898,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>19</v>
@@ -891,10 +909,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C22">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -902,7 +920,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23">
         <v>25</v>
@@ -924,10 +942,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C25">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -982,18 +1000,18 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>42</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1004,81 +1022,102 @@
         <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
         <v>45</v>
       </c>
-      <c r="B34" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="1" t="s">
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>88</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1093,108 +1132,106 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55">
-        <v>3</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>77</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>84</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>83</v>
-      </c>
-      <c r="B59">
-        <v>2</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1204,7 +1241,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1212,302 +1249,362 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C4" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
         <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
-        <v>45815</v>
+        <v>45817</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45815</v>
+        <v>45817</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45814</v>
+        <v>45817</v>
       </c>
       <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45817</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45817</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>73</v>
       </c>
-      <c r="E15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" t="s">
-        <v>73</v>
+      <c r="C18" s="3">
+        <v>45817</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated reports and occupancy for 6.11.25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="115">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/09/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/09/2025)</t>
+    <t>Adoptions (06/10/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/10/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -113,15 +113,6 @@
     <t>2025-06-13</t>
   </si>
   <si>
-    <t>A0058650379</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Treatment, 02</t>
-  </si>
-  <si>
-    <t>2025-06-10</t>
-  </si>
-  <si>
     <t>A0058662816</t>
   </si>
   <si>
@@ -137,15 +128,6 @@
     <t xml:space="preserve">  Cat Treatment, 05 - B</t>
   </si>
   <si>
-    <t>A0058648104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Farm, Farm</t>
-  </si>
-  <si>
-    <t>2025-06-11</t>
-  </si>
-  <si>
     <t>A0058672310</t>
   </si>
   <si>
@@ -155,24 +137,21 @@
     <t>2025-06-16</t>
   </si>
   <si>
-    <t>A0058627436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Multi Animal Holding</t>
-  </si>
-  <si>
     <t>A0058662527</t>
   </si>
   <si>
     <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 1</t>
   </si>
   <si>
-    <t>A0058676024</t>
+    <t>A0058679430</t>
   </si>
   <si>
     <t xml:space="preserve">  Receiving, Receiving</t>
   </si>
   <si>
+    <t>2025-06-17</t>
+  </si>
+  <si>
     <t>AnimalNumber</t>
   </si>
   <si>
@@ -191,79 +170,115 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058360707</t>
-  </si>
-  <si>
-    <t>A0058360718</t>
-  </si>
-  <si>
-    <t>A0058360725</t>
-  </si>
-  <si>
-    <t>A0058668717</t>
-  </si>
-  <si>
-    <t>A0058669677</t>
-  </si>
-  <si>
-    <t>A0058670777</t>
-  </si>
-  <si>
-    <t>A0058670802</t>
-  </si>
-  <si>
-    <t>A0058670807</t>
-  </si>
-  <si>
-    <t>A0058671983</t>
-  </si>
-  <si>
-    <t>A0058672839</t>
-  </si>
-  <si>
-    <t>A0032144299</t>
-  </si>
-  <si>
-    <t>A0058669457</t>
-  </si>
-  <si>
-    <t>A0058669458</t>
-  </si>
-  <si>
-    <t>Rabbit</t>
+    <t>A0057052406</t>
+  </si>
+  <si>
+    <t>A0058621971</t>
+  </si>
+  <si>
+    <t>A0058668403</t>
+  </si>
+  <si>
+    <t>A0058670929</t>
+  </si>
+  <si>
+    <t>A0055794806</t>
+  </si>
+  <si>
+    <t>A0058677023</t>
+  </si>
+  <si>
+    <t>A0058683082</t>
+  </si>
+  <si>
+    <t>A0058676198</t>
+  </si>
+  <si>
+    <t>A0058676199</t>
+  </si>
+  <si>
+    <t>A0058676200</t>
+  </si>
+  <si>
+    <t>A0058676201</t>
+  </si>
+  <si>
+    <t>A0058676202</t>
+  </si>
+  <si>
+    <t>A0058676722</t>
+  </si>
+  <si>
+    <t>A0058679141</t>
+  </si>
+  <si>
+    <t>A0058679149</t>
+  </si>
+  <si>
+    <t>A0058679157</t>
+  </si>
+  <si>
+    <t>A0058682110</t>
+  </si>
+  <si>
+    <t>A0058682112</t>
+  </si>
+  <si>
+    <t>A0058682114</t>
+  </si>
+  <si>
+    <t>A0058682117</t>
+  </si>
+  <si>
+    <t>A0058682119</t>
+  </si>
+  <si>
+    <t>A0058682122</t>
+  </si>
+  <si>
+    <t>A0058682126</t>
+  </si>
+  <si>
+    <t>A0058682129</t>
+  </si>
+  <si>
+    <t>A0058636785</t>
   </si>
   <si>
     <t>Farm Type Fowl</t>
   </si>
   <si>
-    <t>Reptile/Amphibian</t>
-  </si>
-  <si>
-    <t>Clinic</t>
+    <t>Domestic (Cage) Bird</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Return</t>
+  </si>
+  <si>
     <t>Seized / Custody</t>
   </si>
   <si>
     <t>Stray</t>
   </si>
   <si>
-    <t>Retention</t>
+    <t>Transfer In</t>
   </si>
   <si>
     <t>Euthanasia Request - OTC!</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - FIELD!</t>
-  </si>
-  <si>
-    <t>Protective Custody</t>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>Eviction</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
   </si>
   <si>
     <t>No Hold</t>
@@ -272,79 +287,67 @@
     <t>OTC</t>
   </si>
   <si>
-    <t>Abandoned/Dumped Off at SPCA</t>
+    <t>ACO or DCO in County</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
   </si>
   <si>
     <t>Clinic - Retention</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>not counted</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>Return</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
-  </si>
-  <si>
-    <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
@@ -733,7 +736,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -756,7 +759,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -764,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -780,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -796,7 +799,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -820,7 +823,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -836,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -844,7 +847,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -852,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -868,7 +871,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -887,10 +890,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -898,10 +901,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C21">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -909,10 +912,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C22">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -942,10 +945,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="C25">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -989,18 +992,18 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>39</v>
-      </c>
-      <c r="C31" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1011,227 +1014,197 @@
         <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
         <v>43</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>44</v>
       </c>
-      <c r="C33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" t="s">
-        <v>45</v>
+      <c r="A36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>23</v>
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45">
-        <v>2</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>79</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>81</v>
+      </c>
+      <c r="B54">
+        <v>16</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>92</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>77</v>
-      </c>
-      <c r="B57">
-        <v>3</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>86</v>
-      </c>
-      <c r="D62">
-        <v>3</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1241,7 +1214,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1249,362 +1222,562 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
         <v>79</v>
-      </c>
-      <c r="F7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C15" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="3">
-        <v>45817</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" t="s">
-        <v>77</v>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45818</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated load files for 6.13.25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="99">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/11/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/11/2025)</t>
+    <t>Adoptions (06/12/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/12/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,43 +104,25 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>A0058670106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 231, Cage 5</t>
-  </si>
-  <si>
-    <t>2025-06-13</t>
-  </si>
-  <si>
-    <t>A0058662816</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Treatment, 04</t>
-  </si>
-  <si>
-    <t>2025-06-12</t>
-  </si>
-  <si>
-    <t>A0058673429</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Treatment, 05 - B</t>
-  </si>
-  <si>
-    <t>A0058672310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Farm, Stall #3</t>
-  </si>
-  <si>
-    <t>2025-06-16</t>
-  </si>
-  <si>
-    <t>A0058662527</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 1</t>
+    <t>A0058694543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 231, Cage 1</t>
+  </si>
+  <si>
+    <t>2025-06-17</t>
+  </si>
+  <si>
+    <t>A0058698177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 05</t>
+  </si>
+  <si>
+    <t>A0058698188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 02</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -161,18 +143,117 @@
     <t>IntakeGroup</t>
   </si>
   <si>
+    <t>A0058089659</t>
+  </si>
+  <si>
+    <t>A0058579862</t>
+  </si>
+  <si>
+    <t>A0058653404</t>
+  </si>
+  <si>
+    <t>A0058653406</t>
+  </si>
+  <si>
+    <t>A0058655448</t>
+  </si>
+  <si>
+    <t>A0058661818</t>
+  </si>
+  <si>
+    <t>A0058676386</t>
+  </si>
+  <si>
+    <t>A0058688511</t>
+  </si>
+  <si>
+    <t>A0050951954</t>
+  </si>
+  <si>
+    <t>A0058622451</t>
+  </si>
+  <si>
+    <t>A0058640645</t>
+  </si>
+  <si>
+    <t>A0058694278</t>
+  </si>
+  <si>
+    <t>A0058694280</t>
+  </si>
+  <si>
+    <t>A0058694286</t>
+  </si>
+  <si>
+    <t>A0058696537</t>
+  </si>
+  <si>
+    <t>A0058696743</t>
+  </si>
+  <si>
+    <t>A0058696745</t>
+  </si>
+  <si>
+    <t>A0058696755</t>
+  </si>
+  <si>
+    <t>A0058696758</t>
+  </si>
+  <si>
+    <t>A0058697513</t>
+  </si>
+  <si>
+    <t>Rodent</t>
+  </si>
+  <si>
+    <t>Clinic</t>
+  </si>
+  <si>
+    <t>Owner/Guardian Surrender</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Stray</t>
+  </si>
+  <si>
+    <t>Case - Outreach</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Owned 30 Days or Less - OTC!</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>Clinic - Case Assistance - Outreach</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
     <t>Intake Count Summary</t>
   </si>
   <si>
     <t>Transfer In</t>
   </si>
   <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
     <t>Euthanasia Req – Field</t>
   </si>
   <si>
@@ -212,15 +293,6 @@
     <t>Seized - Hoarding</t>
   </si>
   <si>
-    <t>Return</t>
-  </si>
-  <si>
-    <t>Stray</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
     <t>OTC - OS - SAFE</t>
   </si>
   <si>
@@ -234,9 +306,6 @@
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
-  </si>
-  <si>
-    <t>Clinic - Case Assistance - Outreach</t>
   </si>
   <si>
     <t>Clinic - Outreach</t>
@@ -249,6 +318,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -315,12 +387,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -638,7 +711,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -646,7 +719,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -662,7 +735,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>186</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -678,7 +751,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -702,7 +775,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -718,7 +791,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -726,7 +799,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -734,7 +807,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -750,7 +823,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -769,10 +842,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -780,10 +853,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -791,10 +864,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C22">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -802,7 +875,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>25</v>
@@ -824,10 +897,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C25">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -860,189 +933,188 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
         <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
       </c>
       <c r="C30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>31</v>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>23</v>
+      <c r="A35" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>76</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
+        <v>65</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
+        <v>66</v>
+      </c>
+      <c r="B51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
+        <v>75</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
+        <v>74</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1124,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1060,22 +1132,482 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45820</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated morning_email.py to cound If The Fur Fits and Current Fosters differently
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -719,7 +719,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -735,7 +735,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>197</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:2">

</xml_diff>

<commit_message>
Updated reports for 6/17/25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="109">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/12/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/12/2025)</t>
+    <t>Adoptions (06/16/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/16/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,25 +104,40 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>A0058694543</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 231, Cage 1</t>
-  </si>
-  <si>
-    <t>2025-06-17</t>
-  </si>
-  <si>
-    <t>A0058698177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 05</t>
-  </si>
-  <si>
-    <t>A0058698188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 02</t>
+    <t>A0058709950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 235, Cage 2</t>
+  </si>
+  <si>
+    <t>2025-06-19</t>
+  </si>
+  <si>
+    <t>A0058718824</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Treatment, 04</t>
+  </si>
+  <si>
+    <t>2025-06-20</t>
+  </si>
+  <si>
+    <t>A0058716138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 01 - B</t>
+  </si>
+  <si>
+    <t>A0058706705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 2</t>
+  </si>
+  <si>
+    <t>A0058716766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Small Animals &amp; Exotics, Bird Cage 1</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -143,67 +158,76 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058089659</t>
-  </si>
-  <si>
-    <t>A0058579862</t>
-  </si>
-  <si>
-    <t>A0058653404</t>
-  </si>
-  <si>
-    <t>A0058653406</t>
-  </si>
-  <si>
-    <t>A0058655448</t>
-  </si>
-  <si>
-    <t>A0058661818</t>
-  </si>
-  <si>
-    <t>A0058676386</t>
-  </si>
-  <si>
-    <t>A0058688511</t>
-  </si>
-  <si>
-    <t>A0050951954</t>
-  </si>
-  <si>
-    <t>A0058622451</t>
-  </si>
-  <si>
-    <t>A0058640645</t>
-  </si>
-  <si>
-    <t>A0058694278</t>
-  </si>
-  <si>
-    <t>A0058694280</t>
-  </si>
-  <si>
-    <t>A0058694286</t>
-  </si>
-  <si>
-    <t>A0058696537</t>
-  </si>
-  <si>
-    <t>A0058696743</t>
-  </si>
-  <si>
-    <t>A0058696745</t>
-  </si>
-  <si>
-    <t>A0058696755</t>
-  </si>
-  <si>
-    <t>A0058696758</t>
-  </si>
-  <si>
-    <t>A0058697513</t>
-  </si>
-  <si>
-    <t>Rodent</t>
+    <t>A0058223085</t>
+  </si>
+  <si>
+    <t>A0058679860</t>
+  </si>
+  <si>
+    <t>A0058697050</t>
+  </si>
+  <si>
+    <t>A0058694957</t>
+  </si>
+  <si>
+    <t>A0058706029</t>
+  </si>
+  <si>
+    <t>A0058709460</t>
+  </si>
+  <si>
+    <t>A0058717573</t>
+  </si>
+  <si>
+    <t>A0058718209</t>
+  </si>
+  <si>
+    <t>A0058720454</t>
+  </si>
+  <si>
+    <t>A0058720471</t>
+  </si>
+  <si>
+    <t>A0058720491</t>
+  </si>
+  <si>
+    <t>A0058720528</t>
+  </si>
+  <si>
+    <t>A0058716081</t>
+  </si>
+  <si>
+    <t>A0058716470</t>
+  </si>
+  <si>
+    <t>A0058716471</t>
+  </si>
+  <si>
+    <t>A0058717101</t>
+  </si>
+  <si>
+    <t>A0058717112</t>
+  </si>
+  <si>
+    <t>A0058719464</t>
+  </si>
+  <si>
+    <t>A0058719477</t>
+  </si>
+  <si>
+    <t>A0058719482</t>
+  </si>
+  <si>
+    <t>A0058719488</t>
+  </si>
+  <si>
+    <t>A0058716736</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
+  </si>
+  <si>
+    <t>Domestic (Cage) Bird</t>
   </si>
   <si>
     <t>Clinic</t>
@@ -212,100 +236,106 @@
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Seized / Custody</t>
+  </si>
+  <si>
+    <t>Stray</t>
+  </si>
+  <si>
+    <t>Transfer In</t>
+  </si>
+  <si>
+    <t>Retention</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>Cruelty</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>ACO or DCO in County</t>
+  </si>
+  <si>
+    <t>Clinic - Retention</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
     <t>Return</t>
   </si>
   <si>
-    <t>Stray</t>
-  </si>
-  <si>
-    <t>Case - Outreach</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Owned 30 Days or Less - OTC!</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>OTC</t>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
+  </si>
+  <si>
+    <t>Clinic - Case Assistance</t>
   </si>
   <si>
     <t>Clinic - Case Assistance - Outreach</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
-  </si>
-  <si>
-    <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
-  </si>
-  <si>
-    <t>Clinic - Retention</t>
-  </si>
-  <si>
-    <t>Clinic - Case Assistance</t>
   </si>
   <si>
     <t>Clinic - Outreach</t>
@@ -688,7 +718,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -711,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -719,7 +749,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -735,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -751,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -775,7 +805,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -783,7 +813,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -791,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -799,7 +829,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -807,7 +837,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -815,7 +845,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -823,7 +853,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -842,10 +872,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -853,7 +883,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21">
         <v>19</v>
@@ -864,10 +894,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C22">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -875,10 +905,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -889,7 +919,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -897,10 +927,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C25">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -933,188 +963,219 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="1" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>85</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>66</v>
-      </c>
-      <c r="B51">
-        <v>12</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>74</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58">
+        <v>84</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1124,7 +1185,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1132,482 +1193,522 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C17" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="3">
-        <v>45820</v>
+        <v>45824</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45824</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45824</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 6.18.25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/16/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/16/2025)</t>
+    <t>Adoptions (06/17/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/17/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -122,18 +122,21 @@
     <t>2025-06-20</t>
   </si>
   <si>
-    <t>A0058716138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 01 - B</t>
-  </si>
-  <si>
     <t>A0058706705</t>
   </si>
   <si>
     <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 2</t>
   </si>
   <si>
+    <t>A0058727432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 1</t>
+  </si>
+  <si>
+    <t>2025-06-24</t>
+  </si>
+  <si>
     <t>A0058716766</t>
   </si>
   <si>
@@ -158,76 +161,49 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058223085</t>
-  </si>
-  <si>
-    <t>A0058679860</t>
-  </si>
-  <si>
-    <t>A0058697050</t>
-  </si>
-  <si>
-    <t>A0058694957</t>
-  </si>
-  <si>
-    <t>A0058706029</t>
-  </si>
-  <si>
-    <t>A0058709460</t>
-  </si>
-  <si>
-    <t>A0058717573</t>
+    <t>A0058073288</t>
+  </si>
+  <si>
+    <t>A0058671143</t>
+  </si>
+  <si>
+    <t>A0058671146</t>
+  </si>
+  <si>
+    <t>A0058671149</t>
+  </si>
+  <si>
+    <t>A0058671153</t>
+  </si>
+  <si>
+    <t>A0058705115</t>
   </si>
   <si>
     <t>A0058718209</t>
   </si>
   <si>
-    <t>A0058720454</t>
-  </si>
-  <si>
-    <t>A0058720471</t>
-  </si>
-  <si>
-    <t>A0058720491</t>
-  </si>
-  <si>
-    <t>A0058720528</t>
-  </si>
-  <si>
-    <t>A0058716081</t>
-  </si>
-  <si>
-    <t>A0058716470</t>
-  </si>
-  <si>
-    <t>A0058716471</t>
-  </si>
-  <si>
-    <t>A0058717101</t>
-  </si>
-  <si>
-    <t>A0058717112</t>
-  </si>
-  <si>
-    <t>A0058719464</t>
-  </si>
-  <si>
-    <t>A0058719477</t>
-  </si>
-  <si>
-    <t>A0058719482</t>
-  </si>
-  <si>
-    <t>A0058719488</t>
-  </si>
-  <si>
-    <t>A0058716736</t>
-  </si>
-  <si>
-    <t>Rabbit</t>
-  </si>
-  <si>
-    <t>Domestic (Cage) Bird</t>
+    <t>A0058723929</t>
+  </si>
+  <si>
+    <t>A0058728965</t>
+  </si>
+  <si>
+    <t>A0058726103</t>
+  </si>
+  <si>
+    <t>A0058702607</t>
+  </si>
+  <si>
+    <t>A0058728323</t>
+  </si>
+  <si>
+    <t>A0058728669</t>
+  </si>
+  <si>
+    <t>Farm Type Fowl</t>
+  </si>
+  <si>
+    <t>Rodent</t>
   </si>
   <si>
     <t>Clinic</t>
@@ -242,94 +218,94 @@
     <t>Stray</t>
   </si>
   <si>
+    <t>Medical Treatment</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>Cruelty</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
     <t>Transfer In</t>
   </si>
   <si>
-    <t>Retention</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>Cruelty</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>ACO or DCO in County</t>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
   </si>
   <si>
     <t>Clinic - Retention</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>Return</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
-  </si>
-  <si>
-    <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
@@ -741,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -765,7 +741,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -781,7 +757,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -805,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -821,7 +797,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -829,7 +805,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -837,7 +813,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -853,7 +829,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -872,7 +848,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C20">
         <v>28</v>
@@ -883,7 +859,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>19</v>
@@ -894,10 +870,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C22">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -930,7 +906,7 @@
         <v>145</v>
       </c>
       <c r="C25">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -974,7 +950,7 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -985,15 +961,15 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
@@ -1001,7 +977,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>20</v>
@@ -1015,26 +991,20 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>70</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -1042,86 +1012,86 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1129,53 +1099,56 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>101</v>
+        <v>76</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>75</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>84</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1158,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1193,262 +1166,262 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
         <v>76</v>
-      </c>
-      <c r="F3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
         <v>76</v>
-      </c>
-      <c r="F4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
         <v>77</v>
-      </c>
-      <c r="F7" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
         <v>77</v>
-      </c>
-      <c r="F9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
         <v>78</v>
-      </c>
-      <c r="F11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C13" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1459,16 +1432,16 @@
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1479,236 +1452,16 @@
         <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
         <v>74</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>79</v>
-      </c>
-      <c r="F15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="3">
-        <v>45824</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 6.19.25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="98">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/17/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/17/2025)</t>
+    <t>Adoptions (06/18/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/18/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,15 +104,6 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>A0058709950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 235, Cage 2</t>
-  </si>
-  <si>
-    <t>2025-06-19</t>
-  </si>
-  <si>
     <t>A0058718824</t>
   </si>
   <si>
@@ -122,12 +113,6 @@
     <t>2025-06-20</t>
   </si>
   <si>
-    <t>A0058706705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 2</t>
-  </si>
-  <si>
     <t>A0058727432</t>
   </si>
   <si>
@@ -161,52 +146,61 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058073288</t>
-  </si>
-  <si>
-    <t>A0058671143</t>
-  </si>
-  <si>
-    <t>A0058671146</t>
-  </si>
-  <si>
-    <t>A0058671149</t>
-  </si>
-  <si>
-    <t>A0058671153</t>
-  </si>
-  <si>
-    <t>A0058705115</t>
-  </si>
-  <si>
-    <t>A0058718209</t>
-  </si>
-  <si>
-    <t>A0058723929</t>
-  </si>
-  <si>
-    <t>A0058728965</t>
-  </si>
-  <si>
-    <t>A0058726103</t>
-  </si>
-  <si>
-    <t>A0058702607</t>
-  </si>
-  <si>
-    <t>A0058728323</t>
-  </si>
-  <si>
-    <t>A0058728669</t>
-  </si>
-  <si>
-    <t>Farm Type Fowl</t>
-  </si>
-  <si>
-    <t>Rodent</t>
-  </si>
-  <si>
-    <t>Clinic</t>
+    <t>A0058736922</t>
+  </si>
+  <si>
+    <t>A0058737339</t>
+  </si>
+  <si>
+    <t>A0058733210</t>
+  </si>
+  <si>
+    <t>A0058737658</t>
+  </si>
+  <si>
+    <t>A0058732745</t>
+  </si>
+  <si>
+    <t>A0058733446</t>
+  </si>
+  <si>
+    <t>A0058736662</t>
+  </si>
+  <si>
+    <t>A0058738023</t>
+  </si>
+  <si>
+    <t>A0058718199</t>
+  </si>
+  <si>
+    <t>A0058718216</t>
+  </si>
+  <si>
+    <t>A0058718227</t>
+  </si>
+  <si>
+    <t>A0058718231</t>
+  </si>
+  <si>
+    <t>A0058718238</t>
+  </si>
+  <si>
+    <t>A0058718243</t>
+  </si>
+  <si>
+    <t>A0058718252</t>
+  </si>
+  <si>
+    <t>A0058718268</t>
+  </si>
+  <si>
+    <t>A0058718282</t>
+  </si>
+  <si>
+    <t>A0058718292</t>
+  </si>
+  <si>
+    <t>A0058718303</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
@@ -218,88 +212,85 @@
     <t>Stray</t>
   </si>
   <si>
-    <t>Medical Treatment</t>
-  </si>
-  <si>
-    <t>OTC</t>
+    <t>Transfer In</t>
   </si>
   <si>
     <t>Euthanasia Request - OTC!</t>
   </si>
   <si>
+    <t>Evaluation/Poss Adopt - FIELD!</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Rescue Group out of Coalition</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
     <t>DOA</t>
   </si>
   <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>Cruelty</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>Field</t>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
   </si>
   <si>
     <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>Return</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
   </si>
   <si>
     <t>Clinic - Stray</t>
@@ -694,7 +685,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -717,7 +708,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -725,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -741,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -757,7 +748,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -781,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -797,7 +788,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -805,7 +796,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -813,7 +804,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -829,7 +820,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -848,10 +839,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C20">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -859,7 +850,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C21">
         <v>19</v>
@@ -870,10 +861,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -881,10 +872,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C23">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -892,7 +883,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -903,10 +894,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C25">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -953,202 +944,171 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>34</v>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34">
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>23</v>
+      <c r="A35" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
+        <v>75</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>79</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>74</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53">
-        <v>2</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54">
-        <v>4</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>75</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1118,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1166,133 +1126,133 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D6" t="s">
         <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
@@ -1301,167 +1261,267 @@
         <v>69</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
         <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D11" t="s">
         <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45826</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45826</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45826</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45826</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="3">
-        <v>45825</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" t="s">
-        <v>79</v>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45826</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45826</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 6/20/25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/18/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/18/2025)</t>
+    <t>Adoptions (06/19/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/19/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,13 +104,13 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>A0058718824</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Treatment, 04</t>
-  </si>
-  <si>
-    <t>2025-06-20</t>
+    <t>A0058734302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 234, Cage 2</t>
+  </si>
+  <si>
+    <t>2025-06-24</t>
   </si>
   <si>
     <t>A0058727432</t>
@@ -119,15 +119,6 @@
     <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 1</t>
   </si>
   <si>
-    <t>2025-06-24</t>
-  </si>
-  <si>
-    <t>A0058716766</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Small Animals &amp; Exotics, Bird Cage 1</t>
-  </si>
-  <si>
     <t>AnimalNumber</t>
   </si>
   <si>
@@ -146,67 +137,61 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058736922</t>
-  </si>
-  <si>
-    <t>A0058737339</t>
-  </si>
-  <si>
-    <t>A0058733210</t>
-  </si>
-  <si>
-    <t>A0058737658</t>
-  </si>
-  <si>
-    <t>A0058732745</t>
-  </si>
-  <si>
-    <t>A0058733446</t>
-  </si>
-  <si>
-    <t>A0058736662</t>
-  </si>
-  <si>
-    <t>A0058738023</t>
-  </si>
-  <si>
-    <t>A0058718199</t>
-  </si>
-  <si>
-    <t>A0058718216</t>
-  </si>
-  <si>
-    <t>A0058718227</t>
-  </si>
-  <si>
-    <t>A0058718231</t>
-  </si>
-  <si>
-    <t>A0058718238</t>
-  </si>
-  <si>
-    <t>A0058718243</t>
-  </si>
-  <si>
-    <t>A0058718252</t>
-  </si>
-  <si>
-    <t>A0058718268</t>
-  </si>
-  <si>
-    <t>A0058718282</t>
-  </si>
-  <si>
-    <t>A0058718292</t>
-  </si>
-  <si>
-    <t>A0058718303</t>
+    <t>A0051151112</t>
+  </si>
+  <si>
+    <t>A0058737688</t>
+  </si>
+  <si>
+    <t>A0058744626</t>
+  </si>
+  <si>
+    <t>A0058744628</t>
+  </si>
+  <si>
+    <t>A0058744631</t>
+  </si>
+  <si>
+    <t>A0058744636</t>
+  </si>
+  <si>
+    <t>A0058744640</t>
+  </si>
+  <si>
+    <t>A0046108202</t>
+  </si>
+  <si>
+    <t>A0050275902</t>
+  </si>
+  <si>
+    <t>A0052271961</t>
+  </si>
+  <si>
+    <t>A0058741355</t>
+  </si>
+  <si>
+    <t>A0058741358</t>
+  </si>
+  <si>
+    <t>A0058741713</t>
+  </si>
+  <si>
+    <t>A0058741830</t>
+  </si>
+  <si>
+    <t>A0058742495</t>
+  </si>
+  <si>
+    <t>A0058743361</t>
+  </si>
+  <si>
+    <t>A0058690617</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
-    <t>Seized / Custody</t>
+    <t>Return</t>
   </si>
   <si>
     <t>Stray</t>
@@ -221,16 +206,22 @@
     <t>Evaluation/Poss Adopt - FIELD!</t>
   </si>
   <si>
-    <t>Signed Over</t>
+    <t>Owned More than 30 Days - OTC!</t>
+  </si>
+  <si>
+    <t>OTC</t>
   </si>
   <si>
     <t>No Hold</t>
   </si>
   <si>
+    <t>DOA</t>
+  </si>
+  <si>
     <t>Field</t>
   </si>
   <si>
-    <t>Rescue Group out of Coalition</t>
+    <t>SPCA - Other Counties</t>
   </si>
   <si>
     <t>Euthanasia Request</t>
@@ -239,33 +230,30 @@
     <t>Field – OS</t>
   </si>
   <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
     <t>Seized – Signed over</t>
   </si>
   <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
     <t>Seized – Eviction</t>
   </si>
   <si>
@@ -279,9 +267,6 @@
   </si>
   <si>
     <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>Return</t>
   </si>
   <si>
     <t>OTC – OS</t>
@@ -685,7 +670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -708,7 +693,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -716,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -732,7 +717,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -748,7 +733,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -772,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -804,7 +789,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -815,15 +800,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -834,7 +819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -845,7 +830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -853,32 +838,32 @@
         <v>36</v>
       </c>
       <c r="C21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C22">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -889,18 +874,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C25">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -911,7 +896,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -922,7 +907,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -930,185 +915,180 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36">
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1118,7 +1098,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1126,402 +1106,382 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
         <v>65</v>
       </c>
-      <c r="E13" t="s">
-        <v>71</v>
-      </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" t="s">
         <v>65</v>
       </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
         <v>65</v>
       </c>
-      <c r="E16" t="s">
-        <v>71</v>
-      </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45827</v>
+      </c>
+      <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="3">
-        <v>45826</v>
-      </c>
-      <c r="D18" t="s">
-        <v>65</v>
-      </c>
       <c r="E18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" t="s">
         <v>71</v>
-      </c>
-      <c r="F18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="3">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="3">
-        <v>45826</v>
-      </c>
-      <c r="D20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 6/23/25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="122">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/19/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/19/2025)</t>
+    <t>Adoptions (06/20/2025, 6/21/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/20/2025, 6/21/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,6 +104,15 @@
     <t>Review Date</t>
   </si>
   <si>
+    <t>A0058695418</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Adoption Condo Rooms, Rabbitat 1</t>
+  </si>
+  <si>
+    <t>2025-06-26</t>
+  </si>
+  <si>
     <t>A0058734302</t>
   </si>
   <si>
@@ -113,6 +122,15 @@
     <t>2025-06-24</t>
   </si>
   <si>
+    <t>A0035002298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 01 - B</t>
+  </si>
+  <si>
+    <t>No Review Date</t>
+  </si>
+  <si>
     <t>A0058727432</t>
   </si>
   <si>
@@ -137,55 +155,112 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0051151112</t>
-  </si>
-  <si>
-    <t>A0058737688</t>
-  </si>
-  <si>
-    <t>A0058744626</t>
-  </si>
-  <si>
-    <t>A0058744628</t>
-  </si>
-  <si>
-    <t>A0058744631</t>
-  </si>
-  <si>
-    <t>A0058744636</t>
-  </si>
-  <si>
-    <t>A0058744640</t>
-  </si>
-  <si>
-    <t>A0046108202</t>
-  </si>
-  <si>
-    <t>A0050275902</t>
-  </si>
-  <si>
-    <t>A0052271961</t>
-  </si>
-  <si>
-    <t>A0058741355</t>
-  </si>
-  <si>
-    <t>A0058741358</t>
-  </si>
-  <si>
-    <t>A0058741713</t>
-  </si>
-  <si>
-    <t>A0058741830</t>
-  </si>
-  <si>
-    <t>A0058742495</t>
-  </si>
-  <si>
-    <t>A0058743361</t>
-  </si>
-  <si>
-    <t>A0058690617</t>
+    <t>A0058581988</t>
+  </si>
+  <si>
+    <t>A0058727921</t>
+  </si>
+  <si>
+    <t>A0058729123</t>
+  </si>
+  <si>
+    <t>A0058748113</t>
+  </si>
+  <si>
+    <t>A0058748530</t>
+  </si>
+  <si>
+    <t>A0058748533</t>
+  </si>
+  <si>
+    <t>A0058748536</t>
+  </si>
+  <si>
+    <t>A0058748541</t>
+  </si>
+  <si>
+    <t>A0058748559</t>
+  </si>
+  <si>
+    <t>A0058748561</t>
+  </si>
+  <si>
+    <t>A0058748566</t>
+  </si>
+  <si>
+    <t>A0058748569</t>
+  </si>
+  <si>
+    <t>A0058748790</t>
+  </si>
+  <si>
+    <t>A0058748794</t>
+  </si>
+  <si>
+    <t>A0058749076</t>
+  </si>
+  <si>
+    <t>A0058752173</t>
+  </si>
+  <si>
+    <t>A0058755847</t>
+  </si>
+  <si>
+    <t>A0058757630</t>
+  </si>
+  <si>
+    <t>A0058757640</t>
+  </si>
+  <si>
+    <t>A0058758488</t>
+  </si>
+  <si>
+    <t>A0058622436</t>
+  </si>
+  <si>
+    <t>A0058753935</t>
+  </si>
+  <si>
+    <t>A0058753940</t>
+  </si>
+  <si>
+    <t>A0058753950</t>
+  </si>
+  <si>
+    <t>A0058753956</t>
+  </si>
+  <si>
+    <t>A0058753958</t>
+  </si>
+  <si>
+    <t>A0058753963</t>
+  </si>
+  <si>
+    <t>A0058753970</t>
+  </si>
+  <si>
+    <t>A0058753979</t>
+  </si>
+  <si>
+    <t>A0058753987</t>
+  </si>
+  <si>
+    <t>A0058747360</t>
+  </si>
+  <si>
+    <t>A0058747362</t>
+  </si>
+  <si>
+    <t>A0058755856</t>
+  </si>
+  <si>
+    <t>A0058755861</t>
+  </si>
+  <si>
+    <t>A0058757250</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
@@ -194,51 +269,69 @@
     <t>Return</t>
   </si>
   <si>
+    <t>Seized / Custody</t>
+  </si>
+  <si>
     <t>Stray</t>
   </si>
   <si>
     <t>Transfer In</t>
   </si>
   <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
     <t>Euthanasia Request - OTC!</t>
   </si>
   <si>
     <t>Evaluation/Poss Adopt - FIELD!</t>
   </si>
   <si>
-    <t>Owned More than 30 Days - OTC!</t>
-  </si>
-  <si>
     <t>OTC</t>
   </si>
   <si>
+    <t>Euthanasia Request - FIELD!</t>
+  </si>
+  <si>
+    <t>Guardian Surrender - FIELD!</t>
+  </si>
+  <si>
+    <t>Owned 30 Days or Less - OTC!</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
     <t>No Hold</t>
   </si>
   <si>
+    <t>Vet clinic</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
     <t>DOA</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>SPCA - Other Counties</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
     <t>Field – Stray</t>
   </si>
   <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
     <t>Seized – Abandoned</t>
   </si>
   <si>
@@ -251,9 +344,6 @@
     <t>Seized – Hospital</t>
   </si>
   <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
     <t>Seized – Eviction</t>
   </si>
   <si>
@@ -267,9 +357,6 @@
   </si>
   <si>
     <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
   </si>
   <si>
     <t>OTC - OS - SAFE</t>
@@ -670,7 +757,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -693,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -701,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -717,7 +804,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -733,7 +820,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -757,7 +844,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -773,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -781,7 +868,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -797,18 +884,18 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -819,18 +906,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C20">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -838,32 +925,32 @@
         <v>36</v>
       </c>
       <c r="C21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -874,18 +961,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C25">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -896,7 +983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -907,7 +994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -915,180 +1002,217 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35">
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37">
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49">
-        <v>2</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B50">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>97</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1222,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1106,382 +1230,782 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3">
-        <v>45827</v>
+        <v>45829</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45829</v>
+      </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45829</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45829</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="3">
-        <v>45827</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="C22" s="3">
+        <v>45829</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
         <v>68</v>
       </c>
-      <c r="F19" t="s">
-        <v>60</v>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="3">
+        <v>45828</v>
+      </c>
+      <c r="D36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="3">
+        <v>45829</v>
+      </c>
+      <c r="D37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="3">
+        <v>45829</v>
+      </c>
+      <c r="D38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="3">
+        <v>45829</v>
+      </c>
+      <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 6.24.25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="139">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/20/2025, 6/21/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/20/2025, 6/21/2025)</t>
+    <t>Adoptions (06/23/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/23/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -113,30 +113,42 @@
     <t>2025-06-26</t>
   </si>
   <si>
-    <t>A0058734302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 234, Cage 2</t>
+    <t>A0058763771</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 231, Cage 4</t>
+  </si>
+  <si>
+    <t>No Review Date</t>
+  </si>
+  <si>
+    <t>A0035002298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 01 - B</t>
+  </si>
+  <si>
+    <t>A0058727432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Multi Animal Holding</t>
   </si>
   <si>
     <t>2025-06-24</t>
   </si>
   <si>
-    <t>A0035002298</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 01 - B</t>
-  </si>
-  <si>
-    <t>No Review Date</t>
-  </si>
-  <si>
-    <t>A0058727432</t>
+    <t>A0058764920</t>
   </si>
   <si>
     <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 1</t>
   </si>
   <si>
+    <t>A0058765684</t>
+  </si>
+  <si>
+    <t>2025-06-30</t>
+  </si>
+  <si>
     <t>AnimalNumber</t>
   </si>
   <si>
@@ -155,220 +167,259 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058581988</t>
-  </si>
-  <si>
-    <t>A0058727921</t>
-  </si>
-  <si>
-    <t>A0058729123</t>
-  </si>
-  <si>
-    <t>A0058748113</t>
-  </si>
-  <si>
-    <t>A0058748530</t>
-  </si>
-  <si>
-    <t>A0058748533</t>
-  </si>
-  <si>
-    <t>A0058748536</t>
-  </si>
-  <si>
-    <t>A0058748541</t>
-  </si>
-  <si>
-    <t>A0058748559</t>
-  </si>
-  <si>
-    <t>A0058748561</t>
-  </si>
-  <si>
-    <t>A0058748566</t>
-  </si>
-  <si>
-    <t>A0058748569</t>
-  </si>
-  <si>
-    <t>A0058748790</t>
-  </si>
-  <si>
-    <t>A0058748794</t>
-  </si>
-  <si>
-    <t>A0058749076</t>
-  </si>
-  <si>
-    <t>A0058752173</t>
-  </si>
-  <si>
-    <t>A0058755847</t>
-  </si>
-  <si>
-    <t>A0058757630</t>
-  </si>
-  <si>
-    <t>A0058757640</t>
-  </si>
-  <si>
-    <t>A0058758488</t>
-  </si>
-  <si>
-    <t>A0058622436</t>
-  </si>
-  <si>
-    <t>A0058753935</t>
-  </si>
-  <si>
-    <t>A0058753940</t>
-  </si>
-  <si>
-    <t>A0058753950</t>
-  </si>
-  <si>
-    <t>A0058753956</t>
-  </si>
-  <si>
-    <t>A0058753958</t>
-  </si>
-  <si>
-    <t>A0058753963</t>
-  </si>
-  <si>
-    <t>A0058753970</t>
-  </si>
-  <si>
-    <t>A0058753979</t>
-  </si>
-  <si>
-    <t>A0058753987</t>
-  </si>
-  <si>
-    <t>A0058747360</t>
-  </si>
-  <si>
-    <t>A0058747362</t>
-  </si>
-  <si>
-    <t>A0058755856</t>
-  </si>
-  <si>
-    <t>A0058755861</t>
-  </si>
-  <si>
-    <t>A0058757250</t>
+    <t>A0058454216</t>
+  </si>
+  <si>
+    <t>A0058568926</t>
+  </si>
+  <si>
+    <t>A0058763197</t>
+  </si>
+  <si>
+    <t>A0016850435</t>
+  </si>
+  <si>
+    <t>A0047809430</t>
+  </si>
+  <si>
+    <t>A0051707058</t>
+  </si>
+  <si>
+    <t>A0057996204</t>
+  </si>
+  <si>
+    <t>A0057996215</t>
+  </si>
+  <si>
+    <t>A0057996233</t>
+  </si>
+  <si>
+    <t>A0057996245</t>
+  </si>
+  <si>
+    <t>A0058588779</t>
+  </si>
+  <si>
+    <t>A0058729684</t>
+  </si>
+  <si>
+    <t>A0058729698</t>
+  </si>
+  <si>
+    <t>A0058729703</t>
+  </si>
+  <si>
+    <t>A0058729706</t>
+  </si>
+  <si>
+    <t>A0058729710</t>
+  </si>
+  <si>
+    <t>A0058734134</t>
+  </si>
+  <si>
+    <t>A0058734140</t>
+  </si>
+  <si>
+    <t>A0058734147</t>
+  </si>
+  <si>
+    <t>A0058749349</t>
+  </si>
+  <si>
+    <t>A0058763044</t>
+  </si>
+  <si>
+    <t>A0058764550</t>
+  </si>
+  <si>
+    <t>A0058764565</t>
+  </si>
+  <si>
+    <t>A0058765306</t>
+  </si>
+  <si>
+    <t>A0058767718</t>
+  </si>
+  <si>
+    <t>A0058767736</t>
+  </si>
+  <si>
+    <t>A0058763999</t>
+  </si>
+  <si>
+    <t>A0058764006</t>
+  </si>
+  <si>
+    <t>A0058762583</t>
+  </si>
+  <si>
+    <t>A0058762584</t>
+  </si>
+  <si>
+    <t>A0058762585</t>
+  </si>
+  <si>
+    <t>A0058762586</t>
+  </si>
+  <si>
+    <t>A0058762960</t>
+  </si>
+  <si>
+    <t>A0058763173</t>
+  </si>
+  <si>
+    <t>A0058763174</t>
+  </si>
+  <si>
+    <t>A0058763177</t>
+  </si>
+  <si>
+    <t>A0058763180</t>
+  </si>
+  <si>
+    <t>A0058763319</t>
+  </si>
+  <si>
+    <t>A0058763584</t>
+  </si>
+  <si>
+    <t>A0058765957</t>
+  </si>
+  <si>
+    <t>A0058767738</t>
+  </si>
+  <si>
+    <t>A0058764479</t>
   </si>
   <si>
     <t>Rabbit</t>
   </si>
   <si>
+    <t>Rodent</t>
+  </si>
+  <si>
+    <t>Reptile/Amphibian</t>
+  </si>
+  <si>
+    <t>Clinic</t>
+  </si>
+  <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Seized / Custody</t>
+  </si>
+  <si>
+    <t>Stray</t>
+  </si>
+  <si>
+    <t>Transfer In</t>
+  </si>
+  <si>
+    <t>Retention</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Guardian Surrender - FIELD!</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>Guardian Surrender - OTC!</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - FIELD!</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>Born in Care</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>Abandoned by owner - OTC!</t>
+  </si>
+  <si>
+    <t>ACO or DCO in County</t>
+  </si>
+  <si>
+    <t>Clinic - Retention</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
     <t>Return</t>
   </si>
   <si>
-    <t>Seized / Custody</t>
-  </si>
-  <si>
-    <t>Stray</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - FIELD!</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - FIELD!</t>
-  </si>
-  <si>
-    <t>Guardian Surrender - FIELD!</t>
-  </si>
-  <si>
-    <t>Owned 30 Days or Less - OTC!</t>
-  </si>
-  <si>
-    <t>Signed Over</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>Vet clinic</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
     <t>OTC - OS - SAFE</t>
   </si>
   <si>
     <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
-  </si>
-  <si>
-    <t>Clinic - Retention</t>
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
@@ -757,7 +808,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -780,7 +831,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -788,7 +839,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -804,7 +855,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -812,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -820,7 +871,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -844,7 +895,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -860,7 +911,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -868,7 +919,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -892,7 +943,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -911,7 +962,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C20">
         <v>27</v>
@@ -922,10 +973,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -933,10 +984,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C22">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -947,7 +998,7 @@
         <v>30</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -955,7 +1006,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -966,10 +1017,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="C25">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1013,206 +1064,228 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>39</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="1" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38">
+        <v>107</v>
+      </c>
+      <c r="D38">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>118</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40">
-        <v>8</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>116</v>
+      </c>
+      <c r="B42">
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45">
-        <v>6</v>
-      </c>
-      <c r="C45">
-        <v>3</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>110</v>
+        <v>119</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52">
-        <v>6</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>2</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="B54">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1222,7 +1295,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1230,782 +1303,922 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C2" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="C12" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F14" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F17" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C21" s="3">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="3">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F24" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C25" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="C26" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F27" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E28" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D29" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F29" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F30" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E31" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="F31" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="F32" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="F33" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="C34" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E34" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
         <v>20</v>
       </c>
       <c r="C35" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="3">
-        <v>45828</v>
+        <v>45831</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E36" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="F36" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="3">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="F37" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
         <v>20</v>
       </c>
       <c r="C38" s="3">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E38" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="F38" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
         <v>20</v>
       </c>
       <c r="C39" s="3">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="E39" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>86</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="3">
+        <v>45831</v>
+      </c>
+      <c r="D40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="3">
+        <v>45831</v>
+      </c>
+      <c r="D41" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="3">
+        <v>45831</v>
+      </c>
+      <c r="D42" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="3">
+        <v>45831</v>
+      </c>
+      <c r="D43" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="3">
+        <v>45831</v>
+      </c>
+      <c r="D44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="3">
+        <v>45831</v>
+      </c>
+      <c r="D45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="3">
+        <v>45831</v>
+      </c>
+      <c r="D46" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data for 6/26/25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/24/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/24/2025)</t>
+    <t>Adoptions (06/25/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/25/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -128,13 +128,7 @@
     <t xml:space="preserve">  ICU, 01 - B</t>
   </si>
   <si>
-    <t>No Review Date</t>
-  </si>
-  <si>
-    <t>A0058764920</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 1</t>
+    <t>2025-06-26</t>
   </si>
   <si>
     <t>A0058765684</t>
@@ -164,136 +158,97 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058589089</t>
-  </si>
-  <si>
-    <t>A0058718599</t>
-  </si>
-  <si>
-    <t>A0058734634</t>
-  </si>
-  <si>
-    <t>A0058770794</t>
-  </si>
-  <si>
-    <t>A0058772641</t>
-  </si>
-  <si>
-    <t>A0058772686</t>
-  </si>
-  <si>
-    <t>A0058772993</t>
-  </si>
-  <si>
-    <t>A0058775218</t>
-  </si>
-  <si>
-    <t>A0053747735</t>
-  </si>
-  <si>
-    <t>A0058774353</t>
-  </si>
-  <si>
-    <t>A0058770859</t>
-  </si>
-  <si>
-    <t>A0058773648</t>
-  </si>
-  <si>
-    <t>A0058770648</t>
-  </si>
-  <si>
-    <t>Rabbit</t>
-  </si>
-  <si>
-    <t>Rodent</t>
+    <t>A0058779670</t>
+  </si>
+  <si>
+    <t>A0058780889</t>
+  </si>
+  <si>
+    <t>A0058783844</t>
+  </si>
+  <si>
+    <t>A0058780905</t>
+  </si>
+  <si>
+    <t>A0058781169</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Seized / Custody</t>
+  </si>
+  <si>
+    <t>Stray</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Guardian Surrender - OTC!</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Transfer In</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
     <t>Return</t>
-  </si>
-  <si>
-    <t>Seized / Custody</t>
-  </si>
-  <si>
-    <t>Stray</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>Owned More than 30 Days - OTC!</t>
-  </si>
-  <si>
-    <t>Signed Over</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>ACO or DCO in County</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
   </si>
   <si>
     <t>OTC - OS - SAFE</t>
@@ -694,7 +649,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -717,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -725,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -741,7 +696,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -781,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -797,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -805,7 +760,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -829,7 +784,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -848,10 +803,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C20">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -859,10 +814,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C21">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -870,10 +825,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C22">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -903,10 +858,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="C25">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -961,191 +916,171 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
         <v>40</v>
       </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>42</v>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>23</v>
+      <c r="A35" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36">
+        <v>56</v>
+      </c>
+      <c r="B36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>62</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>61</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>77</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1155,7 +1090,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1163,302 +1098,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="3">
-        <v>45832</v>
+        <v>45833</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>45832</v>
+        <v>45833</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
-        <v>45832</v>
+        <v>45833</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45832</v>
+        <v>45833</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45832</v>
+        <v>45833</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
         <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="3">
-        <v>45832</v>
-      </c>
-      <c r="D15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 6.27.25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="117">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/25/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/25/2025)</t>
+    <t>Adoptions (06/26/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/26/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -113,22 +113,19 @@
     <t>2025-06-28</t>
   </si>
   <si>
-    <t>A0058763771</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 231, Cage 4</t>
-  </si>
-  <si>
-    <t>2025-06-27</t>
-  </si>
-  <si>
-    <t>A0035002298</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 01 - B</t>
-  </si>
-  <si>
-    <t>2025-06-26</t>
+    <t>A0058789119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Treatment, B</t>
+  </si>
+  <si>
+    <t>2025-07-01</t>
+  </si>
+  <si>
+    <t>A0058795880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 02</t>
   </si>
   <si>
     <t>A0058765684</t>
@@ -158,60 +155,168 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058779670</t>
-  </si>
-  <si>
-    <t>A0058780889</t>
-  </si>
-  <si>
-    <t>A0058783844</t>
-  </si>
-  <si>
-    <t>A0058780905</t>
-  </si>
-  <si>
-    <t>A0058781169</t>
+    <t>A0057606321</t>
+  </si>
+  <si>
+    <t>A0057606331</t>
+  </si>
+  <si>
+    <t>A0057606333</t>
+  </si>
+  <si>
+    <t>A0058647055</t>
+  </si>
+  <si>
+    <t>A0058757250</t>
+  </si>
+  <si>
+    <t>A0058771476</t>
+  </si>
+  <si>
+    <t>A0058779323</t>
+  </si>
+  <si>
+    <t>A0058787827</t>
+  </si>
+  <si>
+    <t>A0058789307</t>
+  </si>
+  <si>
+    <t>A0058344428</t>
+  </si>
+  <si>
+    <t>A0058703414</t>
+  </si>
+  <si>
+    <t>A0058718252</t>
+  </si>
+  <si>
+    <t>A0058787487</t>
+  </si>
+  <si>
+    <t>A0058787489</t>
+  </si>
+  <si>
+    <t>A0058787491</t>
+  </si>
+  <si>
+    <t>A0058787494</t>
+  </si>
+  <si>
+    <t>A0058787496</t>
+  </si>
+  <si>
+    <t>A0058787499</t>
+  </si>
+  <si>
+    <t>A0058787532</t>
+  </si>
+  <si>
+    <t>A0058792719</t>
+  </si>
+  <si>
+    <t>A0058792732</t>
+  </si>
+  <si>
+    <t>A0058778873</t>
+  </si>
+  <si>
+    <t>A0058787259</t>
+  </si>
+  <si>
+    <t>A0058787263</t>
+  </si>
+  <si>
+    <t>A0058787609</t>
+  </si>
+  <si>
+    <t>A0058790016</t>
+  </si>
+  <si>
+    <t>A0058793704</t>
+  </si>
+  <si>
+    <t>A0058793726</t>
+  </si>
+  <si>
+    <t>A0058793733</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
+  </si>
+  <si>
+    <t>Clinic</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Return</t>
+  </si>
+  <si>
     <t>Seized / Custody</t>
   </si>
   <si>
     <t>Stray</t>
   </si>
   <si>
+    <t>Case - Outreach</t>
+  </si>
+  <si>
     <t>Euthanasia Request - OTC!</t>
   </si>
   <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>Owned 30 Days or Less - OTC!</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>Eviction</t>
+  </si>
+  <si>
+    <t>Cruelty</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>Abandoned by owner - OTC!</t>
+  </si>
+  <si>
+    <t>Clinic - Case Assistance - Outreach</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Transfer In</t>
+  </si>
+  <si>
     <t>DOA</t>
   </si>
   <si>
-    <t>Guardian Surrender - OTC!</t>
-  </si>
-  <si>
-    <t>Signed Over</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
     <t>Euthanasia Req – Field</t>
   </si>
   <si>
@@ -224,18 +329,12 @@
     <t>Seized – Abandoned</t>
   </si>
   <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
     <t>Seized – General</t>
   </si>
   <si>
     <t>Seized – Hospital</t>
   </si>
   <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
     <t>Seized – Police</t>
   </si>
   <si>
@@ -248,9 +347,6 @@
     <t>Seized - Hoarding</t>
   </si>
   <si>
-    <t>Return</t>
-  </si>
-  <si>
     <t>OTC - OS - SAFE</t>
   </si>
   <si>
@@ -264,9 +360,6 @@
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
-  </si>
-  <si>
-    <t>Clinic - Case Assistance - Outreach</t>
   </si>
   <si>
     <t>Clinic - Outreach</t>
@@ -672,7 +765,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -680,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -696,7 +789,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -712,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -736,7 +829,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -744,7 +837,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -752,7 +845,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -760,7 +853,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -768,7 +861,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -784,7 +877,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -803,10 +896,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C20">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -814,10 +907,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C21">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -825,10 +918,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C22">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -836,7 +929,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -847,7 +940,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -858,10 +951,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="C25">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -905,23 +998,23 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>39</v>
-      </c>
-      <c r="C31" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>20</v>
@@ -935,20 +1028,20 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>92</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -956,131 +1049,152 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>96</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>95</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>78</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B52">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53">
         <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>61</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>91</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1090,7 +1204,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1098,122 +1212,622 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3">
-        <v>45833</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>54</v>
       </c>
-      <c r="E6" t="s">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
-        <v>54</v>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45834</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 7.1.25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/27/2025, 06/28/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/27/2025, 06/28/2025)</t>
+    <t>Adoptions (06/30/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (06/30/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -113,19 +113,22 @@
     <t>2025-07-02</t>
   </si>
   <si>
-    <t>A0058795880</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 02</t>
-  </si>
-  <si>
-    <t>2025-07-01</t>
-  </si>
-  <si>
-    <t>A0058796476</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 03 - A</t>
+    <t>A0058812302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 01</t>
+  </si>
+  <si>
+    <t>2025-07-05</t>
+  </si>
+  <si>
+    <t>A0058812861</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 2</t>
+  </si>
+  <si>
+    <t>2025-07-07</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -146,138 +149,84 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058805230</t>
+    <t>A0058563467</t>
+  </si>
+  <si>
+    <t>A0058772179</t>
+  </si>
+  <si>
+    <t>A0058816447</t>
+  </si>
+  <si>
+    <t>A0015599570</t>
   </si>
   <si>
     <t>A0054021734</t>
   </si>
   <si>
-    <t>A0058780847</t>
-  </si>
-  <si>
-    <t>A0058787214</t>
-  </si>
-  <si>
-    <t>A0058790320</t>
-  </si>
-  <si>
-    <t>A0058800447</t>
-  </si>
-  <si>
-    <t>A0058800763</t>
-  </si>
-  <si>
-    <t>A0058803369</t>
-  </si>
-  <si>
-    <t>A0058804124</t>
-  </si>
-  <si>
-    <t>A0058804353</t>
-  </si>
-  <si>
-    <t>A0058805787</t>
-  </si>
-  <si>
-    <t>A0058805800</t>
-  </si>
-  <si>
-    <t>A0058805811</t>
-  </si>
-  <si>
-    <t>A0058373583</t>
-  </si>
-  <si>
-    <t>A0058640973</t>
-  </si>
-  <si>
-    <t>A0058797987</t>
-  </si>
-  <si>
-    <t>A0058798000</t>
-  </si>
-  <si>
-    <t>A0058798054</t>
-  </si>
-  <si>
-    <t>A0058801947</t>
-  </si>
-  <si>
-    <t>A0058801964</t>
-  </si>
-  <si>
-    <t>A0058806595</t>
-  </si>
-  <si>
-    <t>A0040017266</t>
-  </si>
-  <si>
-    <t>A0058790535</t>
-  </si>
-  <si>
-    <t>A0058790545</t>
-  </si>
-  <si>
-    <t>A0058790552</t>
-  </si>
-  <si>
-    <t>A0058790558</t>
-  </si>
-  <si>
-    <t>A0058790560</t>
-  </si>
-  <si>
-    <t>A0058795591</t>
-  </si>
-  <si>
-    <t>A0058796649</t>
-  </si>
-  <si>
-    <t>A0058796651</t>
-  </si>
-  <si>
-    <t>A0058796654</t>
-  </si>
-  <si>
-    <t>A0058796655</t>
-  </si>
-  <si>
-    <t>A0058796658</t>
-  </si>
-  <si>
-    <t>A0058796660</t>
-  </si>
-  <si>
-    <t>A0058796661</t>
-  </si>
-  <si>
-    <t>A0058796664</t>
-  </si>
-  <si>
-    <t>A0058796665</t>
-  </si>
-  <si>
-    <t>A0058797788</t>
-  </si>
-  <si>
-    <t>A0058797907</t>
-  </si>
-  <si>
-    <t>A0058799429</t>
-  </si>
-  <si>
-    <t>A0058799431</t>
-  </si>
-  <si>
-    <t>Mammal</t>
-  </si>
-  <si>
-    <t>Reptile/Amphibian</t>
+    <t>A0058804211</t>
+  </si>
+  <si>
+    <t>A0058811219</t>
+  </si>
+  <si>
+    <t>A0058812472</t>
+  </si>
+  <si>
+    <t>A0058812728</t>
+  </si>
+  <si>
+    <t>A0058813263</t>
+  </si>
+  <si>
+    <t>A0058813495</t>
+  </si>
+  <si>
+    <t>A0058817552</t>
+  </si>
+  <si>
+    <t>A0058501223</t>
+  </si>
+  <si>
+    <t>A0058814043</t>
+  </si>
+  <si>
+    <t>A0058814049</t>
+  </si>
+  <si>
+    <t>A0058814052</t>
+  </si>
+  <si>
+    <t>A0058814056</t>
+  </si>
+  <si>
+    <t>A0058814060</t>
+  </si>
+  <si>
+    <t>A0058817102</t>
+  </si>
+  <si>
+    <t>A0058811036</t>
+  </si>
+  <si>
+    <t>A0058816089</t>
+  </si>
+  <si>
+    <t>A0058811183</t>
+  </si>
+  <si>
+    <t>A0058811207</t>
   </si>
   <si>
     <t>Rabbit</t>
   </si>
   <si>
+    <t>Domestic (Cage) Bird</t>
+  </si>
+  <si>
+    <t>Farm Type Fowl</t>
+  </si>
+  <si>
     <t>Clinic</t>
   </si>
   <si>
@@ -293,16 +242,28 @@
     <t>Stray</t>
   </si>
   <si>
+    <t>Transfer In</t>
+  </si>
+  <si>
+    <t>Retention</t>
+  </si>
+  <si>
     <t>Euthanasia Request - OTC!</t>
   </si>
   <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>Owned 30 Days or Less - OTC!</t>
-  </si>
-  <si>
-    <t>Abandoned</t>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Guardian Surrender - OTC!</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>Guardian Surrender - FIELD!</t>
+  </si>
+  <si>
+    <t>Owned More than 30 Days FIELD!</t>
   </si>
   <si>
     <t>Signed Over</t>
@@ -311,10 +272,13 @@
     <t>Owner died</t>
   </si>
   <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>No Hold</t>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>ACO or DCO in County</t>
+  </si>
+  <si>
+    <t>Clinic - Retention</t>
   </si>
   <si>
     <t>Clinic - Stray</t>
@@ -326,33 +290,27 @@
     <t>OTC – OS</t>
   </si>
   <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
     <t>Seized – Abandoned</t>
   </si>
   <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
     <t>Seized – Cruelty</t>
   </si>
   <si>
@@ -378,9 +336,6 @@
   </si>
   <si>
     <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Clinic - Retention</t>
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
@@ -792,7 +747,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -800,7 +755,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -816,7 +771,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -824,7 +779,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -832,7 +787,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -856,7 +811,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -864,7 +819,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -872,7 +827,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -880,7 +835,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -934,7 +889,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C21">
         <v>21</v>
@@ -945,10 +900,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C22">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -959,7 +914,7 @@
         <v>37</v>
       </c>
       <c r="C23">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -978,10 +933,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C25">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1025,12 +980,12 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>20</v>
@@ -1044,87 +999,96 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>75</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>78</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>94</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>91</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>103</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1132,20 +1096,17 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -1153,42 +1114,39 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B51">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1196,27 +1154,30 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>87</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1226,7 +1187,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1234,902 +1195,522 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
         <v>87</v>
-      </c>
-      <c r="E2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
         <v>88</v>
-      </c>
-      <c r="E4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C16" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C18" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C21" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <v>45836</v>
+        <v>45838</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C23" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="F24" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F25" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C26" s="3">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D27" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D28" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D29" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D30" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D32" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D33" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" t="s">
-        <v>99</v>
-      </c>
-      <c r="F33" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D34" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
         <v>75</v>
-      </c>
-      <c r="B36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" t="s">
-        <v>99</v>
-      </c>
-      <c r="F36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D37" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" t="s">
-        <v>99</v>
-      </c>
-      <c r="F38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D39" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" t="s">
-        <v>99</v>
-      </c>
-      <c r="F39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D40" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40" t="s">
-        <v>99</v>
-      </c>
-      <c r="F40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D41" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" t="s">
-        <v>99</v>
-      </c>
-      <c r="F41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="3">
-        <v>45836</v>
-      </c>
-      <c r="D42" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F42" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D43" t="s">
-        <v>91</v>
-      </c>
-      <c r="E43" t="s">
-        <v>98</v>
-      </c>
-      <c r="F43" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="3">
-        <v>45835</v>
-      </c>
-      <c r="D44" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" t="s">
-        <v>98</v>
-      </c>
-      <c r="F44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="3">
-        <v>45836</v>
-      </c>
-      <c r="D45" t="s">
-        <v>91</v>
-      </c>
-      <c r="E45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated load files for 7.2.25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="110">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (06/30/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (06/30/2025)</t>
+    <t>Adoptions (07/01/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (07/01/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,13 +104,13 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>A0058803379</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 231, Cage 6</t>
-  </si>
-  <si>
-    <t>2025-07-02</t>
+    <t>A0058819245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Adoption Condo Rooms, Rabbitat 2</t>
+  </si>
+  <si>
+    <t>2025-07-08</t>
   </si>
   <si>
     <t>A0058812302</t>
@@ -149,87 +149,90 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058563467</t>
-  </si>
-  <si>
-    <t>A0058772179</t>
-  </si>
-  <si>
-    <t>A0058816447</t>
-  </si>
-  <si>
-    <t>A0015599570</t>
-  </si>
-  <si>
-    <t>A0054021734</t>
-  </si>
-  <si>
-    <t>A0058804211</t>
-  </si>
-  <si>
-    <t>A0058811219</t>
-  </si>
-  <si>
-    <t>A0058812472</t>
-  </si>
-  <si>
-    <t>A0058812728</t>
-  </si>
-  <si>
-    <t>A0058813263</t>
-  </si>
-  <si>
-    <t>A0058813495</t>
-  </si>
-  <si>
-    <t>A0058817552</t>
-  </si>
-  <si>
-    <t>A0058501223</t>
-  </si>
-  <si>
-    <t>A0058814043</t>
-  </si>
-  <si>
-    <t>A0058814049</t>
-  </si>
-  <si>
-    <t>A0058814052</t>
-  </si>
-  <si>
-    <t>A0058814056</t>
-  </si>
-  <si>
-    <t>A0058814060</t>
-  </si>
-  <si>
-    <t>A0058817102</t>
-  </si>
-  <si>
-    <t>A0058811036</t>
-  </si>
-  <si>
-    <t>A0058816089</t>
-  </si>
-  <si>
-    <t>A0058811183</t>
-  </si>
-  <si>
-    <t>A0058811207</t>
+    <t>A0058735803</t>
+  </si>
+  <si>
+    <t>A0058775077</t>
+  </si>
+  <si>
+    <t>A0058811083</t>
+  </si>
+  <si>
+    <t>A0058820045</t>
+  </si>
+  <si>
+    <t>A0058822904</t>
+  </si>
+  <si>
+    <t>A0058822907</t>
+  </si>
+  <si>
+    <t>A0058822909</t>
+  </si>
+  <si>
+    <t>A0058822916</t>
+  </si>
+  <si>
+    <t>A0058301744</t>
+  </si>
+  <si>
+    <t>A0058819858</t>
+  </si>
+  <si>
+    <t>A0058819243</t>
+  </si>
+  <si>
+    <t>A0058819386</t>
+  </si>
+  <si>
+    <t>A0058820115</t>
+  </si>
+  <si>
+    <t>A0058821278</t>
+  </si>
+  <si>
+    <t>A0058821500</t>
+  </si>
+  <si>
+    <t>A0058821514</t>
+  </si>
+  <si>
+    <t>A0058821534</t>
+  </si>
+  <si>
+    <t>A0058821547</t>
+  </si>
+  <si>
+    <t>A0058822625</t>
+  </si>
+  <si>
+    <t>A0058823210</t>
+  </si>
+  <si>
+    <t>A0058823213</t>
+  </si>
+  <si>
+    <t>A0058823216</t>
+  </si>
+  <si>
+    <t>A0058823219</t>
+  </si>
+  <si>
+    <t>A0058815706</t>
+  </si>
+  <si>
+    <t>A0058815714</t>
+  </si>
+  <si>
+    <t>A0058815755</t>
+  </si>
+  <si>
+    <t>A0058815762</t>
   </si>
   <si>
     <t>Rabbit</t>
   </si>
   <si>
-    <t>Domestic (Cage) Bird</t>
-  </si>
-  <si>
-    <t>Farm Type Fowl</t>
-  </si>
-  <si>
-    <t>Clinic</t>
-  </si>
-  <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
@@ -245,97 +248,91 @@
     <t>Transfer In</t>
   </si>
   <si>
-    <t>Retention</t>
+    <t>Evaluation/Poss Adopt - OTC!</t>
   </si>
   <si>
     <t>Euthanasia Request - OTC!</t>
   </si>
   <si>
+    <t>Evaluation/Poss Adopt - FIELD!</t>
+  </si>
+  <si>
+    <t>Medical Treatment - OTC!</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>Feral Cat Focus</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
     <t>DOA</t>
   </si>
   <si>
-    <t>Guardian Surrender - OTC!</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>Guardian Surrender - FIELD!</t>
-  </si>
-  <si>
-    <t>Owned More than 30 Days FIELD!</t>
-  </si>
-  <si>
-    <t>Signed Over</t>
-  </si>
-  <si>
-    <t>Owner died</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>ACO or DCO in County</t>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
   </si>
   <si>
     <t>Clinic - Retention</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
-  </si>
-  <si>
-    <t>Clinic - Medical Treatment</t>
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
@@ -747,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -755,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -771,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -811,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -827,7 +824,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -835,7 +832,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -859,7 +856,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -878,10 +875,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -889,10 +886,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -900,10 +897,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C22">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -911,7 +908,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>26</v>
@@ -922,7 +919,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -933,10 +930,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="C25">
-        <v>218</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -985,7 +982,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>20</v>
@@ -999,125 +996,110 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36">
+        <v>86</v>
+      </c>
+      <c r="C36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44">
-        <v>5</v>
+        <v>88</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50">
+        <v>73</v>
+      </c>
+      <c r="B50">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1125,59 +1107,53 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>87</v>
-      </c>
-      <c r="D56">
-        <v>2</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1163,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1218,19 +1194,19 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1238,19 +1214,19 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1258,19 +1234,19 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1278,19 +1254,19 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1298,19 +1274,19 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1318,19 +1294,19 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1338,19 +1314,19 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
         <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1358,19 +1334,19 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1378,19 +1354,19 @@
         <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1398,19 +1374,19 @@
         <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1418,276 +1394,276 @@
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C13" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
         <v>83</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
         <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
         <v>83</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s">
         <v>83</v>
       </c>
       <c r="F18" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
         <v>83</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D25" t="s">
         <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F25" t="s">
         <v>75</v>
@@ -1695,22 +1671,82 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="3">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F26" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45839</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45839</v>
+      </c>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="3">
+        <v>45839</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 7/7/25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="133">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (07/01/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (07/01/2025)</t>
+    <t>Adoptions (07/03/2025, 07/05/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (07/03/2025, 07/05/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,31 +104,43 @@
     <t>Review Date</t>
   </si>
   <si>
+    <t>A0058840701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 231, Cage 4</t>
+  </si>
+  <si>
+    <t>2025-07-08</t>
+  </si>
+  <si>
+    <t>A0058839495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 234, Cage 6</t>
+  </si>
+  <si>
+    <t>A0058812861</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 2</t>
+  </si>
+  <si>
+    <t>2025-07-07</t>
+  </si>
+  <si>
+    <t>A0058849616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Multi Animal Holding</t>
+  </si>
+  <si>
+    <t>2025-07-11</t>
+  </si>
+  <si>
     <t>A0058819245</t>
   </si>
   <si>
-    <t xml:space="preserve">  Cat Adoption Condo Rooms, Rabbitat 2</t>
-  </si>
-  <si>
-    <t>2025-07-08</t>
-  </si>
-  <si>
-    <t>A0058812302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ICU, 01</t>
-  </si>
-  <si>
-    <t>2025-07-05</t>
-  </si>
-  <si>
-    <t>A0058812861</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Rabbitat 2</t>
-  </si>
-  <si>
-    <t>2025-07-07</t>
+    <t xml:space="preserve">  Small Animals &amp; Exotics, Mammal 4</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -149,88 +161,136 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058735803</t>
-  </si>
-  <si>
-    <t>A0058775077</t>
-  </si>
-  <si>
-    <t>A0058811083</t>
-  </si>
-  <si>
-    <t>A0058820045</t>
-  </si>
-  <si>
-    <t>A0058822904</t>
-  </si>
-  <si>
-    <t>A0058822907</t>
-  </si>
-  <si>
-    <t>A0058822909</t>
-  </si>
-  <si>
-    <t>A0058822916</t>
-  </si>
-  <si>
-    <t>A0058301744</t>
-  </si>
-  <si>
-    <t>A0058819858</t>
-  </si>
-  <si>
-    <t>A0058819243</t>
-  </si>
-  <si>
-    <t>A0058819386</t>
-  </si>
-  <si>
-    <t>A0058820115</t>
-  </si>
-  <si>
-    <t>A0058821278</t>
-  </si>
-  <si>
-    <t>A0058821500</t>
-  </si>
-  <si>
-    <t>A0058821514</t>
-  </si>
-  <si>
-    <t>A0058821534</t>
-  </si>
-  <si>
-    <t>A0058821547</t>
-  </si>
-  <si>
-    <t>A0058822625</t>
-  </si>
-  <si>
-    <t>A0058823210</t>
-  </si>
-  <si>
-    <t>A0058823213</t>
-  </si>
-  <si>
-    <t>A0058823216</t>
-  </si>
-  <si>
-    <t>A0058823219</t>
-  </si>
-  <si>
-    <t>A0058815706</t>
-  </si>
-  <si>
-    <t>A0058815714</t>
-  </si>
-  <si>
-    <t>A0058815755</t>
-  </si>
-  <si>
-    <t>A0058815762</t>
-  </si>
-  <si>
-    <t>Rabbit</t>
+    <t>A0058837698</t>
+  </si>
+  <si>
+    <t>A0054633714</t>
+  </si>
+  <si>
+    <t>A0058797381</t>
+  </si>
+  <si>
+    <t>A0058797603</t>
+  </si>
+  <si>
+    <t>A0058797608</t>
+  </si>
+  <si>
+    <t>A0058797612</t>
+  </si>
+  <si>
+    <t>A0058797613</t>
+  </si>
+  <si>
+    <t>A0058797614</t>
+  </si>
+  <si>
+    <t>A0058797617</t>
+  </si>
+  <si>
+    <t>A0058828034</t>
+  </si>
+  <si>
+    <t>A0058828077</t>
+  </si>
+  <si>
+    <t>A0058829525</t>
+  </si>
+  <si>
+    <t>A0058840714</t>
+  </si>
+  <si>
+    <t>A0058840716</t>
+  </si>
+  <si>
+    <t>A0058846483</t>
+  </si>
+  <si>
+    <t>A0058849219</t>
+  </si>
+  <si>
+    <t>A0055874744</t>
+  </si>
+  <si>
+    <t>A0058421981</t>
+  </si>
+  <si>
+    <t>A0058836708</t>
+  </si>
+  <si>
+    <t>A0058840216</t>
+  </si>
+  <si>
+    <t>A0058840227</t>
+  </si>
+  <si>
+    <t>A0058840242</t>
+  </si>
+  <si>
+    <t>A0058840248</t>
+  </si>
+  <si>
+    <t>A0058840262</t>
+  </si>
+  <si>
+    <t>A0058849570</t>
+  </si>
+  <si>
+    <t>A0058823724</t>
+  </si>
+  <si>
+    <t>A0058823725</t>
+  </si>
+  <si>
+    <t>A0058823726</t>
+  </si>
+  <si>
+    <t>A0058828052</t>
+  </si>
+  <si>
+    <t>A0058828053</t>
+  </si>
+  <si>
+    <t>A0058836765</t>
+  </si>
+  <si>
+    <t>A0058837850</t>
+  </si>
+  <si>
+    <t>A0058838635</t>
+  </si>
+  <si>
+    <t>A0058838653</t>
+  </si>
+  <si>
+    <t>A0058838661</t>
+  </si>
+  <si>
+    <t>A0058838669</t>
+  </si>
+  <si>
+    <t>A0058847120</t>
+  </si>
+  <si>
+    <t>A0058847793</t>
+  </si>
+  <si>
+    <t>A0058848390</t>
+  </si>
+  <si>
+    <t>A0058848924</t>
+  </si>
+  <si>
+    <t>A0058067302</t>
+  </si>
+  <si>
+    <t>A0058838875</t>
+  </si>
+  <si>
+    <t>Domestic (Cage) Bird</t>
+  </si>
+  <si>
+    <t>Clinic</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
@@ -248,54 +308,66 @@
     <t>Transfer In</t>
   </si>
   <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - FIELD!</t>
+  </si>
+  <si>
     <t>Evaluation/Poss Adopt - OTC!</t>
   </si>
   <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - FIELD!</t>
-  </si>
-  <si>
-    <t>Medical Treatment - OTC!</t>
+    <t>Guardian Surrender - OTC!</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Owned More than 30 Days - OTC!</t>
+  </si>
+  <si>
+    <t>Owned 30 Days or Less - OTC!</t>
   </si>
   <si>
     <t>Signed Over</t>
   </si>
   <si>
+    <t>No Hold</t>
+  </si>
+  <si>
     <t>OTC</t>
   </si>
   <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>Feral Cat Focus</t>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>ACO or DCO in County</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
   </si>
   <si>
     <t>OTC – OS</t>
   </si>
   <si>
-    <t>Euthanasia Request</t>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
   </si>
   <si>
     <t>Field – OS</t>
   </si>
   <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
     <t>Seized – Abandoned</t>
   </si>
   <si>
@@ -327,9 +399,6 @@
   </si>
   <si>
     <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
   </si>
   <si>
     <t>Clinic - Retention</t>
@@ -721,7 +790,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -744,7 +813,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -752,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -768,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>188</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -784,7 +853,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -808,7 +877,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -824,7 +893,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -832,7 +901,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -856,7 +925,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -875,10 +944,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C20">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -886,10 +955,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -897,10 +966,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C22">
-        <v>129</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -908,10 +977,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C23">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -919,10 +988,10 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -930,10 +999,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="C25">
-        <v>202</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -966,194 +1035,234 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
         <v>35</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>101</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>110</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>114</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>113</v>
+      </c>
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>75</v>
-      </c>
-      <c r="B51">
-        <v>12</v>
-      </c>
-      <c r="D51">
-        <v>2</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>93</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
       </c>
       <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>95</v>
+      </c>
+      <c r="B53">
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>112</v>
+      </c>
+      <c r="B54">
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>109</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1163,7 +1272,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1171,582 +1280,922 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45839</v>
+        <v>45843</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3">
-        <v>45839</v>
+        <v>45843</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="F22" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="F24" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C26" s="3">
-        <v>45839</v>
+        <v>45843</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="F26" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="F27" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="F28" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="3">
-        <v>45839</v>
+        <v>45841</v>
       </c>
       <c r="D29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
         <v>76</v>
       </c>
-      <c r="E29" t="s">
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D31" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D34" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D36" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" t="s">
+        <v>106</v>
+      </c>
+      <c r="F37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D39" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
         <v>84</v>
       </c>
-      <c r="F29" t="s">
-        <v>76</v>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="3">
+        <v>45843</v>
+      </c>
+      <c r="D40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" t="s">
+        <v>105</v>
+      </c>
+      <c r="F40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="3">
+        <v>45843</v>
+      </c>
+      <c r="D41" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="3">
+        <v>45843</v>
+      </c>
+      <c r="D42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="3">
+        <v>45843</v>
+      </c>
+      <c r="D43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="3">
+        <v>45843</v>
+      </c>
+      <c r="D44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" t="s">
+        <v>106</v>
+      </c>
+      <c r="F44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D45" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" t="s">
+        <v>108</v>
+      </c>
+      <c r="F45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="3">
+        <v>45841</v>
+      </c>
+      <c r="D46" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 7/10/25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="102">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (07/08/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (07/08/2025)</t>
+    <t>Adoptions (07/09/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (07/09/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -140,91 +140,133 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058742107</t>
-  </si>
-  <si>
-    <t>A0058811636</t>
-  </si>
-  <si>
-    <t>A0058819189</t>
-  </si>
-  <si>
-    <t>A0058836833</t>
-  </si>
-  <si>
-    <t>A0058862207</t>
-  </si>
-  <si>
-    <t>A0058864061</t>
-  </si>
-  <si>
-    <t>A0058864064</t>
-  </si>
-  <si>
-    <t>A0058864066</t>
-  </si>
-  <si>
-    <t>A0058864067</t>
-  </si>
-  <si>
-    <t>A0058864070</t>
-  </si>
-  <si>
-    <t>A0058864072</t>
-  </si>
-  <si>
-    <t>A0058866048</t>
-  </si>
-  <si>
-    <t>Rodent</t>
+    <t>A0056924261</t>
+  </si>
+  <si>
+    <t>A0058832269</t>
+  </si>
+  <si>
+    <t>A0058862375</t>
+  </si>
+  <si>
+    <t>A0058872179</t>
+  </si>
+  <si>
+    <t>A0058872186</t>
+  </si>
+  <si>
+    <t>A0058873095</t>
+  </si>
+  <si>
+    <t>A0058865640</t>
+  </si>
+  <si>
+    <t>A0058871542</t>
+  </si>
+  <si>
+    <t>A0058872784</t>
+  </si>
+  <si>
+    <t>A0058872788</t>
+  </si>
+  <si>
+    <t>A0058872790</t>
+  </si>
+  <si>
+    <t>A0058872792</t>
+  </si>
+  <si>
+    <t>A0058872796</t>
+  </si>
+  <si>
+    <t>A0058872798</t>
+  </si>
+  <si>
+    <t>A0058872803</t>
+  </si>
+  <si>
+    <t>A0058872805</t>
+  </si>
+  <si>
+    <t>A0058872807</t>
+  </si>
+  <si>
+    <t>A0058872864</t>
+  </si>
+  <si>
+    <t>A0058872867</t>
+  </si>
+  <si>
+    <t>A0058874744</t>
+  </si>
+  <si>
+    <t>A0058874847</t>
+  </si>
+  <si>
+    <t>A0058874851</t>
+  </si>
+  <si>
+    <t>A0058874852</t>
+  </si>
+  <si>
+    <t>A0058874853</t>
+  </si>
+  <si>
+    <t>A0058874855</t>
+  </si>
+  <si>
+    <t>A0058875207</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Seized / Custody</t>
+  </si>
+  <si>
     <t>Stray</t>
   </si>
   <si>
+    <t>Guardian Surrender - OTC!</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - FIELD!</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Abandoned</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
     <t>Transfer In</t>
   </si>
   <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>ACO or DCO in County</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
     <t>Euthanasia Request</t>
   </si>
   <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
     <t>Field – Stray</t>
   </si>
   <si>
     <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
   </si>
   <si>
     <t>Seized – Cruelty</t>
@@ -678,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -702,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -710,7 +752,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -718,7 +760,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -726,7 +768,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -742,7 +784,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -758,7 +800,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -766,7 +808,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -774,7 +816,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -782,7 +824,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -790,7 +832,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -809,10 +851,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -831,10 +873,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C22">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -842,7 +884,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C23">
         <v>27</v>
@@ -853,10 +895,10 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -864,10 +906,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C25">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -905,7 +947,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>20</v>
@@ -919,155 +961,158 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>73</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>77</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>78</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B50">
-        <v>2</v>
-      </c>
-      <c r="C50">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D50">
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1077,7 +1122,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1108,19 +1153,19 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1131,16 +1176,16 @@
         <v>21</v>
       </c>
       <c r="C3" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1148,19 +1193,19 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1168,19 +1213,19 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1191,176 +1236,436 @@
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C10" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C11" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C12" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C13" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C14" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>56</v>
       </c>
-      <c r="E14" t="s">
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
         <v>61</v>
       </c>
-      <c r="F14" t="s">
-        <v>56</v>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45847</v>
+      </c>
+      <c r="D27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 7/11/25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (07/09/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (07/09/2025)</t>
+    <t>Adoptions (07/10/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (07/10/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,6 +104,15 @@
     <t>Review Date</t>
   </si>
   <si>
+    <t>A0058881800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Adoption Condo Rooms, Rabbitat 2</t>
+  </si>
+  <si>
+    <t>2025-07-16</t>
+  </si>
+  <si>
     <t>A0058862316</t>
   </si>
   <si>
@@ -122,6 +131,24 @@
     <t>2025-07-11</t>
   </si>
   <si>
+    <t>A0058883107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Multi Animal Holding</t>
+  </si>
+  <si>
+    <t>A0058883828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Receiving, Receiving</t>
+  </si>
+  <si>
+    <t>2025-07-15</t>
+  </si>
+  <si>
+    <t>A0058886564</t>
+  </si>
+  <si>
     <t>AnimalNumber</t>
   </si>
   <si>
@@ -140,147 +167,180 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0056924261</t>
-  </si>
-  <si>
-    <t>A0058832269</t>
-  </si>
-  <si>
-    <t>A0058862375</t>
-  </si>
-  <si>
-    <t>A0058872179</t>
-  </si>
-  <si>
-    <t>A0058872186</t>
-  </si>
-  <si>
-    <t>A0058873095</t>
-  </si>
-  <si>
-    <t>A0058865640</t>
-  </si>
-  <si>
-    <t>A0058871542</t>
-  </si>
-  <si>
-    <t>A0058872784</t>
-  </si>
-  <si>
-    <t>A0058872788</t>
-  </si>
-  <si>
-    <t>A0058872790</t>
-  </si>
-  <si>
-    <t>A0058872792</t>
-  </si>
-  <si>
-    <t>A0058872796</t>
-  </si>
-  <si>
-    <t>A0058872798</t>
-  </si>
-  <si>
-    <t>A0058872803</t>
-  </si>
-  <si>
-    <t>A0058872805</t>
-  </si>
-  <si>
-    <t>A0058872807</t>
-  </si>
-  <si>
-    <t>A0058872864</t>
-  </si>
-  <si>
-    <t>A0058872867</t>
-  </si>
-  <si>
-    <t>A0058874744</t>
-  </si>
-  <si>
-    <t>A0058874847</t>
-  </si>
-  <si>
-    <t>A0058874851</t>
-  </si>
-  <si>
-    <t>A0058874852</t>
-  </si>
-  <si>
-    <t>A0058874853</t>
-  </si>
-  <si>
-    <t>A0058874855</t>
-  </si>
-  <si>
-    <t>A0058875207</t>
+    <t>A0057606326</t>
+  </si>
+  <si>
+    <t>A0057606328</t>
+  </si>
+  <si>
+    <t>A0057606329</t>
+  </si>
+  <si>
+    <t>A0058829471</t>
+  </si>
+  <si>
+    <t>A0058829474</t>
+  </si>
+  <si>
+    <t>A0058847947</t>
+  </si>
+  <si>
+    <t>A0058878916</t>
+  </si>
+  <si>
+    <t>A0058884237</t>
+  </si>
+  <si>
+    <t>A0021403555</t>
+  </si>
+  <si>
+    <t>A0054196266</t>
+  </si>
+  <si>
+    <t>A0058639310</t>
+  </si>
+  <si>
+    <t>A0056617154</t>
+  </si>
+  <si>
+    <t>A0058880548</t>
+  </si>
+  <si>
+    <t>A0058880579</t>
+  </si>
+  <si>
+    <t>A0058880606</t>
+  </si>
+  <si>
+    <t>A0058884959</t>
+  </si>
+  <si>
+    <t>A0058873067</t>
+  </si>
+  <si>
+    <t>A0058873074</t>
+  </si>
+  <si>
+    <t>A0058873076</t>
+  </si>
+  <si>
+    <t>A0058878498</t>
+  </si>
+  <si>
+    <t>A0058880145</t>
+  </si>
+  <si>
+    <t>A0058883197</t>
+  </si>
+  <si>
+    <t>A0058883204</t>
+  </si>
+  <si>
+    <t>A0058883212</t>
+  </si>
+  <si>
+    <t>Domestic (Cage) Bird</t>
   </si>
   <si>
     <t>Rabbit</t>
   </si>
   <si>
+    <t>Reptile/Amphibian</t>
+  </si>
+  <si>
+    <t>Clinic</t>
+  </si>
+  <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Return</t>
+  </si>
+  <si>
     <t>Seized / Custody</t>
   </si>
   <si>
     <t>Stray</t>
   </si>
   <si>
-    <t>Guardian Surrender - OTC!</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - FIELD!</t>
+    <t>Transfer In</t>
+  </si>
+  <si>
+    <t>Case - Outreach</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>Owned 30 Days or Less - OTC!</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Protective Custody</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>ACO or DCO in County</t>
+  </si>
+  <si>
+    <t>Clinic - Case Assistance - Outreach</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>not counted</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
   </si>
   <si>
     <t>DOA</t>
   </si>
   <si>
-    <t>Abandoned</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
     <t>Euthanasia Req – Field</t>
   </si>
   <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
     <t>Seized – Abandoned</t>
   </si>
   <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
     <t>Seized – Cruelty</t>
   </si>
   <si>
     <t>Seized – General</t>
   </si>
   <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
     <t>Seized – Eviction</t>
   </si>
   <si>
@@ -296,9 +356,6 @@
     <t>Seized - Hoarding</t>
   </si>
   <si>
-    <t>Return</t>
-  </si>
-  <si>
     <t>OTC - OS - SAFE</t>
   </si>
   <si>
@@ -312,9 +369,6 @@
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
-  </si>
-  <si>
-    <t>Clinic - Case Assistance - Outreach</t>
   </si>
   <si>
     <t>Clinic - Outreach</t>
@@ -697,7 +751,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -720,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -728,7 +782,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -744,7 +798,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -760,7 +814,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -784,7 +838,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -800,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -808,7 +862,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -824,18 +878,18 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -846,18 +900,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -868,51 +922,51 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C22">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C23">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C25">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -923,7 +977,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -934,7 +988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -945,174 +999,230 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="1" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
-      <c r="C39">
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50">
-        <v>11</v>
-      </c>
-      <c r="D50">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>79</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>81</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>101</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>94</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1122,7 +1232,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1130,542 +1240,562 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C14" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C15" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C16" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="F22" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="C23" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C27" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45848</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files for 7/15/25
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="116">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (07/10/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (07/10/2025)</t>
+    <t>Adoptions (07/14/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (07/14/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -113,40 +113,13 @@
     <t>2025-07-16</t>
   </si>
   <si>
-    <t>A0058862316</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 231, Cage 6</t>
-  </si>
-  <si>
-    <t>2025-07-12</t>
-  </si>
-  <si>
-    <t>A0058849616</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Lindsey's Office, Room 159, Lindsey's Office 159</t>
-  </si>
-  <si>
-    <t>2025-07-11</t>
-  </si>
-  <si>
-    <t>A0058883107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Multi-Animal Holding, Room 229, Multi Animal Holding</t>
-  </si>
-  <si>
-    <t>A0058883828</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Receiving, Receiving</t>
-  </si>
-  <si>
-    <t>2025-07-15</t>
-  </si>
-  <si>
-    <t>A0058886564</t>
+    <t>A0058888487</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Treatment, 02</t>
+  </si>
+  <si>
+    <t>2025-07-18</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -167,85 +140,112 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0057606326</t>
-  </si>
-  <si>
-    <t>A0057606328</t>
-  </si>
-  <si>
-    <t>A0057606329</t>
-  </si>
-  <si>
-    <t>A0058829471</t>
-  </si>
-  <si>
-    <t>A0058829474</t>
-  </si>
-  <si>
-    <t>A0058847947</t>
-  </si>
-  <si>
-    <t>A0058878916</t>
-  </si>
-  <si>
-    <t>A0058884237</t>
-  </si>
-  <si>
-    <t>A0021403555</t>
-  </si>
-  <si>
-    <t>A0054196266</t>
-  </si>
-  <si>
-    <t>A0058639310</t>
-  </si>
-  <si>
-    <t>A0056617154</t>
-  </si>
-  <si>
-    <t>A0058880548</t>
-  </si>
-  <si>
-    <t>A0058880579</t>
-  </si>
-  <si>
-    <t>A0058880606</t>
-  </si>
-  <si>
-    <t>A0058884959</t>
-  </si>
-  <si>
-    <t>A0058873067</t>
-  </si>
-  <si>
-    <t>A0058873074</t>
-  </si>
-  <si>
-    <t>A0058873076</t>
-  </si>
-  <si>
-    <t>A0058878498</t>
-  </si>
-  <si>
-    <t>A0058880145</t>
-  </si>
-  <si>
-    <t>A0058883197</t>
-  </si>
-  <si>
-    <t>A0058883204</t>
-  </si>
-  <si>
-    <t>A0058883212</t>
-  </si>
-  <si>
-    <t>Domestic (Cage) Bird</t>
+    <t>A0058645169</t>
+  </si>
+  <si>
+    <t>A0058658142</t>
+  </si>
+  <si>
+    <t>A0058867235</t>
+  </si>
+  <si>
+    <t>A0058894633</t>
+  </si>
+  <si>
+    <t>A0058901666</t>
+  </si>
+  <si>
+    <t>A0058902147</t>
+  </si>
+  <si>
+    <t>A0058902362</t>
+  </si>
+  <si>
+    <t>A0058903821</t>
+  </si>
+  <si>
+    <t>A0058906248</t>
+  </si>
+  <si>
+    <t>A0058906254</t>
+  </si>
+  <si>
+    <t>A0058902017</t>
+  </si>
+  <si>
+    <t>A0058905000</t>
+  </si>
+  <si>
+    <t>A0010646211</t>
+  </si>
+  <si>
+    <t>A0058854358</t>
+  </si>
+  <si>
+    <t>A0058854359</t>
+  </si>
+  <si>
+    <t>A0058887121</t>
+  </si>
+  <si>
+    <t>A0058887122</t>
+  </si>
+  <si>
+    <t>A0058901767</t>
+  </si>
+  <si>
+    <t>A0058901783</t>
+  </si>
+  <si>
+    <t>A0058901787</t>
+  </si>
+  <si>
+    <t>A0058901794</t>
+  </si>
+  <si>
+    <t>A0058901853</t>
+  </si>
+  <si>
+    <t>A0058901926</t>
+  </si>
+  <si>
+    <t>A0058901929</t>
+  </si>
+  <si>
+    <t>A0058901930</t>
+  </si>
+  <si>
+    <t>A0058901931</t>
+  </si>
+  <si>
+    <t>A0058901979</t>
+  </si>
+  <si>
+    <t>A0058902702</t>
+  </si>
+  <si>
+    <t>A0058903437</t>
+  </si>
+  <si>
+    <t>A0058904179</t>
+  </si>
+  <si>
+    <t>A0058904643</t>
+  </si>
+  <si>
+    <t>A0058904859</t>
+  </si>
+  <si>
+    <t>A0058904578</t>
+  </si>
+  <si>
+    <t>A0058904579</t>
   </si>
   <si>
     <t>Rabbit</t>
   </si>
   <si>
-    <t>Reptile/Amphibian</t>
+    <t>Rodent</t>
   </si>
   <si>
     <t>Clinic</t>
@@ -254,121 +254,109 @@
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Seized / Custody</t>
+  </si>
+  <si>
+    <t>Stray</t>
+  </si>
+  <si>
+    <t>Transfer In</t>
+  </si>
+  <si>
+    <t>Retention</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>DOA</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>Born in Care</t>
+  </si>
+  <si>
+    <t>ACO or DCO in County</t>
+  </si>
+  <si>
+    <t>Clinic - Retention</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
     <t>Return</t>
   </si>
   <si>
-    <t>Seized / Custody</t>
-  </si>
-  <si>
-    <t>Stray</t>
-  </si>
-  <si>
-    <t>Transfer In</t>
-  </si>
-  <si>
-    <t>Case - Outreach</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>Owned 30 Days or Less - OTC!</t>
-  </si>
-  <si>
-    <t>Signed Over</t>
-  </si>
-  <si>
-    <t>Hospital</t>
-  </si>
-  <si>
-    <t>Protective Custody</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>ACO or DCO in County</t>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>Clinic - Case Assistance</t>
   </si>
   <si>
     <t>Clinic - Case Assistance - Outreach</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>not counted</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>DOA</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
-  </si>
-  <si>
-    <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
-  </si>
-  <si>
-    <t>Clinic - Retention</t>
-  </si>
-  <si>
-    <t>Clinic - Case Assistance</t>
   </si>
   <si>
     <t>Clinic - Outreach</t>
@@ -751,7 +739,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -774,7 +762,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -798,7 +786,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -814,7 +802,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -838,7 +826,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -846,7 +834,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -854,7 +842,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -862,7 +850,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -870,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -878,18 +866,18 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -900,73 +888,73 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C22">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C23">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C25">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -977,7 +965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -988,7 +976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -999,138 +987,108 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39">
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>108</v>
       </c>
@@ -1142,87 +1100,70 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>80</v>
+      </c>
+      <c r="B50">
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>94</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>79</v>
-      </c>
-      <c r="B53">
-        <v>3</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B54">
-        <v>5</v>
-      </c>
-      <c r="D54">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55">
-        <v>3</v>
+        <v>91</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>94</v>
-      </c>
-      <c r="B61">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +1173,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1240,113 +1181,113 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D2" t="s">
         <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D3" t="s">
         <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D4" t="s">
         <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D5" t="s">
         <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D6" t="s">
         <v>78</v>
@@ -1355,38 +1296,38 @@
         <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D7" t="s">
         <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D8" t="s">
         <v>78</v>
@@ -1395,18 +1336,18 @@
         <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="C9" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D9" t="s">
         <v>78</v>
@@ -1415,58 +1356,58 @@
         <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C10" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C11" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D12" t="s">
         <v>79</v>
@@ -1475,58 +1416,58 @@
         <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D14" t="s">
         <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D15" t="s">
         <v>80</v>
@@ -1535,18 +1476,18 @@
         <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D16" t="s">
         <v>80</v>
@@ -1555,247 +1496,407 @@
         <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D17" t="s">
         <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="3">
-        <v>45848</v>
+        <v>45852</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F28" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="3">
+        <v>45852</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45852</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45852</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45852</v>
+      </c>
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45852</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="3">
+        <v>45852</v>
+      </c>
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="3">
+        <v>45852</v>
+      </c>
+      <c r="D35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="3">
+        <v>45852</v>
+      </c>
+      <c r="D36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated files for 7/16
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="111">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (07/14/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (07/14/2025)</t>
+    <t>Adoptions (07/15/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (07/15/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -113,6 +113,15 @@
     <t>2025-07-16</t>
   </si>
   <si>
+    <t>A0058909086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 235, Cage 2</t>
+  </si>
+  <si>
+    <t>2025-07-19</t>
+  </si>
+  <si>
     <t>A0058888487</t>
   </si>
   <si>
@@ -122,6 +131,27 @@
     <t>2025-07-18</t>
   </si>
   <si>
+    <t>A0058905650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Foster Care Room, 06</t>
+  </si>
+  <si>
+    <t>A0058909081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ICU, 04 - A</t>
+  </si>
+  <si>
+    <t>A0058909084</t>
+  </si>
+  <si>
+    <t>A0058914774</t>
+  </si>
+  <si>
+    <t>A0058914782</t>
+  </si>
+  <si>
     <t>AnimalNumber</t>
   </si>
   <si>
@@ -140,120 +170,66 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0058645169</t>
-  </si>
-  <si>
-    <t>A0058658142</t>
-  </si>
-  <si>
-    <t>A0058867235</t>
-  </si>
-  <si>
-    <t>A0058894633</t>
-  </si>
-  <si>
-    <t>A0058901666</t>
-  </si>
-  <si>
-    <t>A0058902147</t>
-  </si>
-  <si>
-    <t>A0058902362</t>
-  </si>
-  <si>
-    <t>A0058903821</t>
-  </si>
-  <si>
-    <t>A0058906248</t>
-  </si>
-  <si>
-    <t>A0058906254</t>
-  </si>
-  <si>
-    <t>A0058902017</t>
-  </si>
-  <si>
-    <t>A0058905000</t>
-  </si>
-  <si>
-    <t>A0010646211</t>
-  </si>
-  <si>
-    <t>A0058854358</t>
-  </si>
-  <si>
-    <t>A0058854359</t>
-  </si>
-  <si>
-    <t>A0058887121</t>
-  </si>
-  <si>
-    <t>A0058887122</t>
-  </si>
-  <si>
-    <t>A0058901767</t>
-  </si>
-  <si>
-    <t>A0058901783</t>
-  </si>
-  <si>
-    <t>A0058901787</t>
-  </si>
-  <si>
-    <t>A0058901794</t>
-  </si>
-  <si>
-    <t>A0058901853</t>
-  </si>
-  <si>
-    <t>A0058901926</t>
-  </si>
-  <si>
-    <t>A0058901929</t>
-  </si>
-  <si>
-    <t>A0058901930</t>
-  </si>
-  <si>
-    <t>A0058901931</t>
-  </si>
-  <si>
-    <t>A0058901979</t>
-  </si>
-  <si>
-    <t>A0058902702</t>
-  </si>
-  <si>
-    <t>A0058903437</t>
-  </si>
-  <si>
-    <t>A0058904179</t>
-  </si>
-  <si>
-    <t>A0058904643</t>
-  </si>
-  <si>
-    <t>A0058904859</t>
-  </si>
-  <si>
-    <t>A0058904578</t>
-  </si>
-  <si>
-    <t>A0058904579</t>
-  </si>
-  <si>
-    <t>Rabbit</t>
-  </si>
-  <si>
-    <t>Rodent</t>
-  </si>
-  <si>
-    <t>Clinic</t>
+    <t>A0058878747</t>
+  </si>
+  <si>
+    <t>A0058911345</t>
+  </si>
+  <si>
+    <t>A0058911363</t>
+  </si>
+  <si>
+    <t>A0058913920</t>
+  </si>
+  <si>
+    <t>A0039918688</t>
+  </si>
+  <si>
+    <t>A0058041269</t>
+  </si>
+  <si>
+    <t>A0058465907</t>
+  </si>
+  <si>
+    <t>A0058733210</t>
+  </si>
+  <si>
+    <t>A0031109282</t>
+  </si>
+  <si>
+    <t>A0058910423</t>
+  </si>
+  <si>
+    <t>A0058914263</t>
+  </si>
+  <si>
+    <t>A0058914271</t>
+  </si>
+  <si>
+    <t>A0058914274</t>
+  </si>
+  <si>
+    <t>A0058914281</t>
+  </si>
+  <si>
+    <t>A0058914310</t>
+  </si>
+  <si>
+    <t>A0058909286</t>
+  </si>
+  <si>
+    <t>A0058911566</t>
+  </si>
+  <si>
+    <t>A0058913557</t>
   </si>
   <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Return</t>
+  </si>
+  <si>
     <t>Seized / Custody</t>
   </si>
   <si>
@@ -263,94 +239,103 @@
     <t>Transfer In</t>
   </si>
   <si>
-    <t>Retention</t>
-  </si>
-  <si>
     <t>Euthanasia Request - OTC!</t>
   </si>
   <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - FIELD!</t>
+  </si>
+  <si>
+    <t>Owned More than 30 Days - OTC!</t>
+  </si>
+  <si>
+    <t>Owned 30 Days or Less - OTC!</t>
+  </si>
+  <si>
+    <t>Cruelty</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>Abandoned</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>Feral Cat Focus</t>
+  </si>
+  <si>
+    <t>Rescue Group out of Coalition</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>Seized – Cruelty</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Seized – Abandoned</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
   </si>
   <si>
     <t>DOA</t>
   </si>
   <si>
-    <t>Signed Over</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>Born in Care</t>
-  </si>
-  <si>
-    <t>ACO or DCO in County</t>
+    <t>Euthanasia Req – Field</t>
+  </si>
+  <si>
+    <t>Seized – General</t>
+  </si>
+  <si>
+    <t>Seized – Hospital</t>
+  </si>
+  <si>
+    <t>Seized – Eviction</t>
+  </si>
+  <si>
+    <t>Seized – Police</t>
+  </si>
+  <si>
+    <t>Seized – Owner Died</t>
+  </si>
+  <si>
+    <t>Seized – Order Violation</t>
+  </si>
+  <si>
+    <t>Seized - Hoarding</t>
+  </si>
+  <si>
+    <t>OTC - OS - SAFE</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>Clinic - Stray</t>
   </si>
   <si>
     <t>Clinic - Retention</t>
-  </si>
-  <si>
-    <t>Clinic - Stray</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Euthanasia Req – Field</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
-    <t>Seized – Abandoned</t>
-  </si>
-  <si>
-    <t>Seized – Cruelty</t>
-  </si>
-  <si>
-    <t>Seized – General</t>
-  </si>
-  <si>
-    <t>Seized – Hospital</t>
-  </si>
-  <si>
-    <t>Seized – Eviction</t>
-  </si>
-  <si>
-    <t>Seized – Police</t>
-  </si>
-  <si>
-    <t>Seized – Owner Died</t>
-  </si>
-  <si>
-    <t>Seized – Order Violation</t>
-  </si>
-  <si>
-    <t>Seized - Hoarding</t>
-  </si>
-  <si>
-    <t>Return</t>
-  </si>
-  <si>
-    <t>OTC - OS - SAFE</t>
-  </si>
-  <si>
-    <t>Clinic - Medical Treatment</t>
   </si>
   <si>
     <t>Clinic - Case Assistance</t>
@@ -739,7 +724,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -762,7 +747,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -786,7 +771,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>221</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -802,7 +787,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -810,7 +795,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -834,7 +819,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -850,7 +835,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -858,7 +843,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -866,18 +851,18 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -888,73 +873,73 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C22">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C25">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -965,7 +950,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -976,7 +961,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -987,183 +972,255 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33">
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>91</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1173,7 +1230,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1181,722 +1238,502 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45853</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
         <v>78</v>
       </c>
-      <c r="E9" t="s">
-        <v>84</v>
-      </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" s="3">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" t="s">
-        <v>89</v>
-      </c>
-      <c r="F27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D28" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30" t="s">
-        <v>88</v>
-      </c>
-      <c r="F30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D33" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" t="s">
-        <v>88</v>
-      </c>
-      <c r="F33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
         <v>73</v>
-      </c>
-      <c r="B35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" t="s">
-        <v>90</v>
-      </c>
-      <c r="F35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="3">
-        <v>45852</v>
-      </c>
-      <c r="D36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" t="s">
-        <v>90</v>
-      </c>
-      <c r="F36" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Morning Email - includes RTO and Transfer Out now
</commit_message>
<xml_diff>
--- a/MorningEmail/morning_report.xlsx
+++ b/MorningEmail/morning_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="123">
   <si>
     <t>Outcomes</t>
   </si>
@@ -23,10 +23,10 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Adoptions (08/04/2025)</t>
-  </si>
-  <si>
-    <t>If The Fur Fits (08/04/2025)</t>
+    <t>Adoptions (08/07/2025)</t>
+  </si>
+  <si>
+    <t>If The Fur Fits (08/07/2025)</t>
   </si>
   <si>
     <t>Stage</t>
@@ -104,13 +104,19 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>A0059038375</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Cat Isolation 231, Cage 1</t>
-  </si>
-  <si>
-    <t>2025-08-08</t>
+    <t>A0059063708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Isolation 231, Cage 4</t>
+  </si>
+  <si>
+    <t>2025-08-12</t>
+  </si>
+  <si>
+    <t>A0059067638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cat Treatment, 02</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -131,162 +137,213 @@
     <t>IntakeGroup</t>
   </si>
   <si>
-    <t>A0059025461</t>
-  </si>
-  <si>
-    <t>A0059033852</t>
-  </si>
-  <si>
-    <t>A0059038749</t>
-  </si>
-  <si>
-    <t>A0059039044</t>
-  </si>
-  <si>
-    <t>A0059039294</t>
-  </si>
-  <si>
-    <t>A0059039328</t>
-  </si>
-  <si>
-    <t>A0059039330</t>
-  </si>
-  <si>
-    <t>A0059039333</t>
-  </si>
-  <si>
-    <t>A0059039335</t>
-  </si>
-  <si>
-    <t>A0059039336</t>
-  </si>
-  <si>
-    <t>A0059039338</t>
-  </si>
-  <si>
-    <t>A0059039342</t>
-  </si>
-  <si>
-    <t>A0059040430</t>
-  </si>
-  <si>
-    <t>A0059041812</t>
-  </si>
-  <si>
-    <t>A0059043156</t>
-  </si>
-  <si>
-    <t>A0059043163</t>
-  </si>
-  <si>
-    <t>A0059038318</t>
-  </si>
-  <si>
-    <t>A0059038323</t>
-  </si>
-  <si>
-    <t>A0059040144</t>
-  </si>
-  <si>
-    <t>A0059041027</t>
-  </si>
-  <si>
-    <t>A0059041034</t>
-  </si>
-  <si>
-    <t>A0059041041</t>
-  </si>
-  <si>
-    <t>A0059041047</t>
-  </si>
-  <si>
-    <t>A0059041268</t>
-  </si>
-  <si>
-    <t>A0059042285</t>
-  </si>
-  <si>
-    <t>A0059042651</t>
-  </si>
-  <si>
-    <t>A0059042657</t>
-  </si>
-  <si>
-    <t>A0058552576</t>
-  </si>
-  <si>
-    <t>A0059038225</t>
+    <t>A0058788854</t>
+  </si>
+  <si>
+    <t>A0058788856</t>
+  </si>
+  <si>
+    <t>A0058981309</t>
+  </si>
+  <si>
+    <t>A0059054979</t>
+  </si>
+  <si>
+    <t>A0059067064</t>
+  </si>
+  <si>
+    <t>A0058825550</t>
+  </si>
+  <si>
+    <t>A0058825557</t>
+  </si>
+  <si>
+    <t>A0058825574</t>
+  </si>
+  <si>
+    <t>A0059012295</t>
+  </si>
+  <si>
+    <t>A0059012299</t>
+  </si>
+  <si>
+    <t>A0059012303</t>
+  </si>
+  <si>
+    <t>A0059012312</t>
+  </si>
+  <si>
+    <t>A0059019355</t>
+  </si>
+  <si>
+    <t>A0059019358</t>
+  </si>
+  <si>
+    <t>A0059019360</t>
+  </si>
+  <si>
+    <t>A0059032790</t>
+  </si>
+  <si>
+    <t>A0059046186</t>
+  </si>
+  <si>
+    <t>A0059062251</t>
+  </si>
+  <si>
+    <t>A0059063264</t>
+  </si>
+  <si>
+    <t>A0059063506</t>
+  </si>
+  <si>
+    <t>A0059065774</t>
+  </si>
+  <si>
+    <t>A0059066187</t>
+  </si>
+  <si>
+    <t>A0059068106</t>
+  </si>
+  <si>
+    <t>A0058999721</t>
+  </si>
+  <si>
+    <t>A0059067070</t>
+  </si>
+  <si>
+    <t>A0059067074</t>
+  </si>
+  <si>
+    <t>A0059067078</t>
+  </si>
+  <si>
+    <t>A0059067081</t>
+  </si>
+  <si>
+    <t>A0059067084</t>
+  </si>
+  <si>
+    <t>A0059067086</t>
+  </si>
+  <si>
+    <t>A0059067089</t>
+  </si>
+  <si>
+    <t>A0059067091</t>
+  </si>
+  <si>
+    <t>A0059067095</t>
+  </si>
+  <si>
+    <t>A0059067099</t>
+  </si>
+  <si>
+    <t>A0059067103</t>
+  </si>
+  <si>
+    <t>A0059067112</t>
+  </si>
+  <si>
+    <t>A0059067121</t>
+  </si>
+  <si>
+    <t>A0059042672</t>
+  </si>
+  <si>
+    <t>A0059065918</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
   </si>
   <si>
     <t>Rodent</t>
   </si>
   <si>
+    <t>Clinic</t>
+  </si>
+  <si>
     <t>Owner/Guardian Surrender</t>
   </si>
   <si>
+    <t>Return</t>
+  </si>
+  <si>
     <t>Seized / Custody</t>
   </si>
   <si>
     <t>Stray</t>
   </si>
   <si>
+    <t>Retention</t>
+  </si>
+  <si>
+    <t>Medical Treatment</t>
+  </si>
+  <si>
+    <t>Outreach</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - FIELD!</t>
+  </si>
+  <si>
+    <t>Evaluation/Poss Adopt - OTC!</t>
+  </si>
+  <si>
+    <t>Euthanasia Request - OTC!</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Owned 30 Days or Less - OTC!</t>
+  </si>
+  <si>
+    <t>Signed Over</t>
+  </si>
+  <si>
+    <t>No Hold</t>
+  </si>
+  <si>
+    <t>Clinic - Retention</t>
+  </si>
+  <si>
+    <t>Clinic - Medical Treatment</t>
+  </si>
+  <si>
+    <t>Clinic - Outreach</t>
+  </si>
+  <si>
+    <t>Field – OS</t>
+  </si>
+  <si>
+    <t>OTC – OS</t>
+  </si>
+  <si>
+    <t>Euthanasia Request</t>
+  </si>
+  <si>
+    <t>Seized – Signed over</t>
+  </si>
+  <si>
+    <t>Field – Stray</t>
+  </si>
+  <si>
+    <t>Intake Count Summary</t>
+  </si>
+  <si>
     <t>Transfer In</t>
   </si>
   <si>
-    <t>Euthanasia Request - OTC!</t>
-  </si>
-  <si>
-    <t>Evaluation/Poss Adopt - OTC!</t>
-  </si>
-  <si>
-    <t>Euthanasia Request - FIELD!</t>
-  </si>
-  <si>
-    <t>Born in Care</t>
-  </si>
-  <si>
     <t>DOA</t>
   </si>
   <si>
-    <t>Signed Over</t>
-  </si>
-  <si>
-    <t>No Hold</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>Feral Cat Focus</t>
-  </si>
-  <si>
-    <t>ACO or DCO in County</t>
-  </si>
-  <si>
-    <t>Euthanasia Request</t>
-  </si>
-  <si>
-    <t>OTC – OS</t>
-  </si>
-  <si>
     <t>Euthanasia Req – Field</t>
   </si>
   <si>
-    <t>not counted</t>
-  </si>
-  <si>
-    <t>Seized – Signed over</t>
-  </si>
-  <si>
-    <t>Intake Count Summary</t>
-  </si>
-  <si>
-    <t>Field – Stray</t>
-  </si>
-  <si>
-    <t>Field – OS</t>
-  </si>
-  <si>
     <t>Seized – Abandoned</t>
   </si>
   <si>
@@ -314,28 +371,16 @@
     <t>Seized - Hoarding</t>
   </si>
   <si>
-    <t>Return</t>
-  </si>
-  <si>
     <t>OTC - OS - SAFE</t>
   </si>
   <si>
-    <t>Clinic - Medical Treatment</t>
-  </si>
-  <si>
     <t>Clinic - Stray</t>
   </si>
   <si>
-    <t>Clinic - Retention</t>
-  </si>
-  <si>
     <t>Clinic - Case Assistance</t>
   </si>
   <si>
     <t>Clinic - Case Assistance - Outreach</t>
-  </si>
-  <si>
-    <t>Clinic - Outreach</t>
   </si>
   <si>
     <t>Boarder</t>
@@ -715,7 +760,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -738,7 +783,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -746,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -762,7 +807,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>255</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -778,7 +823,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -786,7 +831,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -802,7 +847,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -818,7 +863,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -826,7 +871,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -842,7 +887,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -850,7 +895,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -869,10 +914,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C20">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -880,10 +925,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C21">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -891,10 +936,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -902,10 +947,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C23">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -913,10 +958,10 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -924,10 +969,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="C25">
-        <v>302</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -952,177 +997,203 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="1" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32">
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33">
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35">
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>107</v>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1132,7 +1203,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1140,622 +1211,862 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="C2" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C3" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C22" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="F22" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C26" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
         <v>20</v>
       </c>
       <c r="C30" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
       </c>
       <c r="C31" s="3">
-        <v>45873</v>
+        <v>45876</v>
       </c>
       <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
         <v>71</v>
       </c>
-      <c r="E31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" t="s">
-        <v>71</v>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D34" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D37" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="3">
+        <v>45876</v>
+      </c>
+      <c r="D43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>